<commit_message>
Updated Box Scores, Standings, Playoffs
Data Input to EOD 4/18/24
Scores, Offense, Goalies for first 4 games
</commit_message>
<xml_diff>
--- a/2024/Playoffs/Brackets.xlsx
+++ b/2024/Playoffs/Brackets.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Bracket" sheetId="2" r:id="rId1"/>
-    <sheet name="Matchups" sheetId="3" r:id="rId2"/>
+    <sheet name="Matchups" sheetId="3" r:id="rId1"/>
+    <sheet name="Bracket" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="51">
   <si>
     <t>Eastern Conference Playoff Teams</t>
   </si>
@@ -185,7 +185,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -487,73 +487,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -565,8 +517,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -577,41 +580,38 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -893,16 +893,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="37.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="60"/>
+      <c r="G11" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="59"/>
+      <c r="C13" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="59"/>
+      <c r="E13" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="59"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="59"/>
+      <c r="C16" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="59"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="59"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="59"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H44" s="2"/>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H45" s="2"/>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="48" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H49" s="2"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G51" s="2"/>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G53" s="2"/>
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="L55" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C16:D16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AU26" sqref="AU26:BA26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="12.7109375" style="33" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="20" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="22.5703125" style="1" customWidth="1"/>
@@ -930,138 +1257,139 @@
     <col min="39" max="39" width="22.140625" style="1" customWidth="1"/>
     <col min="40" max="40" width="9.140625" style="1"/>
     <col min="41" max="41" width="22.140625" style="1" customWidth="1"/>
-    <col min="42" max="48" width="9.140625" style="1"/>
-    <col min="49" max="49" width="21.28515625" style="1" customWidth="1"/>
+    <col min="42" max="47" width="9.140625" style="1"/>
+    <col min="48" max="48" width="10.28515625" style="1" customWidth="1"/>
+    <col min="49" max="49" width="23.140625" style="1" customWidth="1"/>
     <col min="50" max="50" width="9.140625" style="1"/>
-    <col min="51" max="51" width="20.42578125" style="1" customWidth="1"/>
+    <col min="51" max="51" width="23.140625" style="1" customWidth="1"/>
     <col min="52" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="28"/>
-      <c r="Z1" s="26" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="52"/>
+      <c r="Z1" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="28"/>
-      <c r="AF1" s="26" t="s">
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="52"/>
+      <c r="AF1" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="28"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="51"/>
+      <c r="AN1" s="51"/>
+      <c r="AO1" s="51"/>
+      <c r="AP1" s="51"/>
+      <c r="AQ1" s="51"/>
+      <c r="AR1" s="51"/>
+      <c r="AS1" s="51"/>
+      <c r="AT1" s="51"/>
+      <c r="AU1" s="51"/>
+      <c r="AV1" s="51"/>
+      <c r="AW1" s="51"/>
+      <c r="AX1" s="51"/>
+      <c r="AY1" s="51"/>
+      <c r="AZ1" s="51"/>
+      <c r="BA1" s="52"/>
     </row>
     <row r="2" spans="1:53" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
-      <c r="M2" s="20" t="s">
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="56"/>
+      <c r="M2" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="22"/>
-      <c r="AI2" s="20" t="s">
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="56"/>
+      <c r="AI2" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
-      <c r="AL2" s="21"/>
-      <c r="AM2" s="21"/>
-      <c r="AN2" s="21"/>
-      <c r="AO2" s="22"/>
-      <c r="AU2" s="20" t="s">
+      <c r="AJ2" s="55"/>
+      <c r="AK2" s="55"/>
+      <c r="AL2" s="55"/>
+      <c r="AM2" s="55"/>
+      <c r="AN2" s="55"/>
+      <c r="AO2" s="56"/>
+      <c r="AU2" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="AV2" s="21"/>
-      <c r="AW2" s="21"/>
-      <c r="AX2" s="21"/>
-      <c r="AY2" s="21"/>
-      <c r="AZ2" s="21"/>
-      <c r="BA2" s="22"/>
+      <c r="AV2" s="55"/>
+      <c r="AW2" s="55"/>
+      <c r="AX2" s="55"/>
+      <c r="AY2" s="55"/>
+      <c r="AZ2" s="55"/>
+      <c r="BA2" s="56"/>
     </row>
     <row r="3" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="AI3" s="19" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="AI3" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="AJ3" s="19"/>
-      <c r="AK3" s="19"/>
-      <c r="AL3" s="19"/>
-      <c r="AM3" s="19"/>
-      <c r="AN3" s="19"/>
-      <c r="AO3" s="19"/>
-      <c r="AU3" s="19" t="s">
+      <c r="AJ3" s="43"/>
+      <c r="AK3" s="43"/>
+      <c r="AL3" s="43"/>
+      <c r="AM3" s="43"/>
+      <c r="AN3" s="43"/>
+      <c r="AO3" s="43"/>
+      <c r="AU3" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="AV3" s="19"/>
-      <c r="AW3" s="19"/>
-      <c r="AX3" s="19"/>
-      <c r="AY3" s="19"/>
-      <c r="AZ3" s="19"/>
-      <c r="BA3" s="19"/>
+      <c r="AV3" s="43"/>
+      <c r="AW3" s="43"/>
+      <c r="AX3" s="43"/>
+      <c r="AY3" s="43"/>
+      <c r="AZ3" s="43"/>
+      <c r="BA3" s="43"/>
     </row>
     <row r="4" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1079,15 +1407,15 @@
       <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="41"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="46"/>
       <c r="AI4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1135,7 +1463,9 @@
       <c r="A5" s="7">
         <v>1</v>
       </c>
-      <c r="B5" s="49"/>
+      <c r="B5" s="30">
+        <v>45403</v>
+      </c>
       <c r="C5" s="10" t="s">
         <v>16</v>
       </c>
@@ -1145,31 +1475,31 @@
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="5"/>
-      <c r="M5" s="38" t="s">
+      <c r="M5" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="38" t="s">
+      <c r="N5" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="38" t="s">
+      <c r="O5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="38" t="s">
+      <c r="P5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="38" t="s">
+      <c r="Q5" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="R5" s="38" t="s">
+      <c r="R5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="S5" s="38" t="s">
+      <c r="S5" s="25" t="s">
         <v>25</v>
       </c>
       <c r="AI5" s="7">
         <v>1</v>
       </c>
-      <c r="AJ5" s="49"/>
+      <c r="AJ5" s="30"/>
       <c r="AK5" s="10"/>
       <c r="AL5" s="11"/>
       <c r="AM5" s="10"/>
@@ -1178,8 +1508,12 @@
       <c r="AU5" s="7">
         <v>1</v>
       </c>
-      <c r="AV5" s="49"/>
-      <c r="AW5" s="10"/>
+      <c r="AV5" s="30">
+        <v>45403</v>
+      </c>
+      <c r="AW5" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="AX5" s="11"/>
       <c r="AY5" s="10" t="s">
         <v>13</v>
@@ -1191,7 +1525,9 @@
       <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="50"/>
+      <c r="B6" s="31">
+        <v>45405</v>
+      </c>
       <c r="C6" s="12" t="s">
         <v>16</v>
       </c>
@@ -1204,7 +1540,7 @@
       <c r="M6" s="7">
         <v>1</v>
       </c>
-      <c r="N6" s="36"/>
+      <c r="N6" s="23"/>
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="10"/>
@@ -1213,7 +1549,7 @@
       <c r="AI6" s="8">
         <v>2</v>
       </c>
-      <c r="AJ6" s="50"/>
+      <c r="AJ6" s="31"/>
       <c r="AK6" s="12"/>
       <c r="AL6" s="13"/>
       <c r="AM6" s="12"/>
@@ -1222,8 +1558,12 @@
       <c r="AU6" s="8">
         <v>2</v>
       </c>
-      <c r="AV6" s="50"/>
-      <c r="AW6" s="12"/>
+      <c r="AV6" s="31">
+        <v>45405</v>
+      </c>
+      <c r="AW6" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="AX6" s="13"/>
       <c r="AY6" s="12" t="s">
         <v>13</v>
@@ -1235,7 +1575,9 @@
       <c r="A7" s="8">
         <v>3</v>
       </c>
-      <c r="B7" s="50"/>
+      <c r="B7" s="31">
+        <v>45408</v>
+      </c>
       <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
@@ -1249,7 +1591,7 @@
       <c r="M7" s="8">
         <v>2</v>
       </c>
-      <c r="N7" s="37"/>
+      <c r="N7" s="24"/>
       <c r="O7" s="12"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="12"/>
@@ -1258,7 +1600,7 @@
       <c r="AI7" s="8">
         <v>3</v>
       </c>
-      <c r="AJ7" s="50"/>
+      <c r="AJ7" s="31"/>
       <c r="AK7" s="12"/>
       <c r="AL7" s="13"/>
       <c r="AM7" s="12"/>
@@ -1267,12 +1609,16 @@
       <c r="AU7" s="8">
         <v>3</v>
       </c>
-      <c r="AV7" s="50"/>
+      <c r="AV7" s="31">
+        <v>45408</v>
+      </c>
       <c r="AW7" s="12" t="s">
         <v>13</v>
       </c>
       <c r="AX7" s="13"/>
-      <c r="AY7" s="12"/>
+      <c r="AY7" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="AZ7" s="13"/>
       <c r="BA7" s="16"/>
     </row>
@@ -1280,7 +1626,9 @@
       <c r="A8" s="8">
         <v>4</v>
       </c>
-      <c r="B8" s="50"/>
+      <c r="B8" s="31">
+        <v>45410</v>
+      </c>
       <c r="C8" s="12" t="s">
         <v>10</v>
       </c>
@@ -1290,13 +1638,13 @@
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="16"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
       <c r="M8" s="8">
         <v>3</v>
       </c>
-      <c r="N8" s="37"/>
+      <c r="N8" s="24"/>
       <c r="O8" s="12"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="12"/>
@@ -1305,24 +1653,28 @@
       <c r="AI8" s="8">
         <v>4</v>
       </c>
-      <c r="AJ8" s="56"/>
-      <c r="AK8" s="53"/>
-      <c r="AL8" s="54"/>
-      <c r="AM8" s="53"/>
-      <c r="AN8" s="54"/>
-      <c r="AO8" s="55"/>
-      <c r="AQ8" s="23"/>
-      <c r="AR8" s="23"/>
-      <c r="AS8" s="23"/>
+      <c r="AJ8" s="37"/>
+      <c r="AK8" s="34"/>
+      <c r="AL8" s="35"/>
+      <c r="AM8" s="34"/>
+      <c r="AN8" s="35"/>
+      <c r="AO8" s="36"/>
+      <c r="AQ8" s="42"/>
+      <c r="AR8" s="42"/>
+      <c r="AS8" s="42"/>
       <c r="AU8" s="8">
         <v>4</v>
       </c>
-      <c r="AV8" s="50"/>
+      <c r="AV8" s="31">
+        <v>45410</v>
+      </c>
       <c r="AW8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="AX8" s="13"/>
-      <c r="AY8" s="12"/>
+      <c r="AY8" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="AZ8" s="13"/>
       <c r="BA8" s="16"/>
     </row>
@@ -1330,7 +1682,7 @@
       <c r="A9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="50"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="12" t="s">
         <v>16</v>
       </c>
@@ -1345,7 +1697,7 @@
       <c r="M9" s="8">
         <v>4</v>
       </c>
-      <c r="N9" s="37"/>
+      <c r="N9" s="24"/>
       <c r="O9" s="12"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="12"/>
@@ -1354,7 +1706,7 @@
       <c r="AI9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AJ9" s="50"/>
+      <c r="AJ9" s="31"/>
       <c r="AK9" s="12"/>
       <c r="AL9" s="13"/>
       <c r="AM9" s="12"/>
@@ -1366,8 +1718,10 @@
       <c r="AU9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AV9" s="50"/>
-      <c r="AW9" s="12"/>
+      <c r="AV9" s="31"/>
+      <c r="AW9" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="AX9" s="13"/>
       <c r="AY9" s="12" t="s">
         <v>13</v>
@@ -1379,7 +1733,7 @@
       <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="50"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="12" t="s">
         <v>10</v>
       </c>
@@ -1393,7 +1747,7 @@
       <c r="M10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N10" s="37"/>
+      <c r="N10" s="24"/>
       <c r="O10" s="12"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="12"/>
@@ -1402,7 +1756,7 @@
       <c r="AI10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AJ10" s="50"/>
+      <c r="AJ10" s="31"/>
       <c r="AK10" s="12"/>
       <c r="AL10" s="13"/>
       <c r="AM10" s="12"/>
@@ -1414,12 +1768,14 @@
       <c r="AU10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AV10" s="50"/>
+      <c r="AV10" s="31"/>
       <c r="AW10" s="12" t="s">
         <v>13</v>
       </c>
       <c r="AX10" s="13"/>
-      <c r="AY10" s="12"/>
+      <c r="AY10" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="AZ10" s="13"/>
       <c r="BA10" s="16"/>
     </row>
@@ -1427,7 +1783,7 @@
       <c r="A11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="51"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="14" t="s">
         <v>16</v>
       </c>
@@ -1441,7 +1797,7 @@
       <c r="M11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N11" s="37"/>
+      <c r="N11" s="24"/>
       <c r="O11" s="12"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="12"/>
@@ -1450,7 +1806,7 @@
       <c r="AI11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AJ11" s="51"/>
+      <c r="AJ11" s="32"/>
       <c r="AK11" s="14"/>
       <c r="AL11" s="15"/>
       <c r="AM11" s="14"/>
@@ -1462,8 +1818,10 @@
       <c r="AU11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AV11" s="51"/>
-      <c r="AW11" s="14"/>
+      <c r="AV11" s="32"/>
+      <c r="AW11" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="AX11" s="15"/>
       <c r="AY11" s="14" t="s">
         <v>13</v>
@@ -1472,96 +1830,96 @@
       <c r="BA11" s="6"/>
     </row>
     <row r="12" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
       <c r="L12" s="12"/>
       <c r="M12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="N12" s="37"/>
+      <c r="N12" s="24"/>
       <c r="O12" s="12"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="12"/>
       <c r="R12" s="13"/>
       <c r="S12" s="16"/>
-      <c r="AI12" s="19" t="s">
+      <c r="AI12" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AJ12" s="19"/>
-      <c r="AK12" s="19"/>
-      <c r="AL12" s="19"/>
-      <c r="AM12" s="19"/>
-      <c r="AN12" s="19"/>
-      <c r="AO12" s="19"/>
+      <c r="AJ12" s="43"/>
+      <c r="AK12" s="43"/>
+      <c r="AL12" s="43"/>
+      <c r="AM12" s="43"/>
+      <c r="AN12" s="43"/>
+      <c r="AO12" s="43"/>
       <c r="AQ12" s="12"/>
       <c r="AR12" s="17"/>
       <c r="AS12" s="17"/>
-      <c r="AU12" s="19" t="s">
+      <c r="AU12" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AV12" s="19"/>
-      <c r="AW12" s="19"/>
-      <c r="AX12" s="19"/>
-      <c r="AY12" s="19"/>
-      <c r="AZ12" s="19"/>
-      <c r="BA12" s="19"/>
+      <c r="AV12" s="43"/>
+      <c r="AW12" s="43"/>
+      <c r="AX12" s="43"/>
+      <c r="AY12" s="43"/>
+      <c r="AZ12" s="43"/>
+      <c r="BA12" s="43"/>
     </row>
     <row r="13" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L13" s="12"/>
-      <c r="M13" s="39" t="s">
+      <c r="M13" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="40"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="40"/>
-      <c r="S13" s="41"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="46"/>
       <c r="AQ13" s="12"/>
       <c r="AR13" s="17"/>
       <c r="AS13" s="17"/>
     </row>
     <row r="14" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="AN14" s="23"/>
-      <c r="AO14" s="23"/>
-      <c r="AP14" s="23"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+      <c r="AN14" s="42"/>
+      <c r="AO14" s="42"/>
+      <c r="AP14" s="42"/>
       <c r="AQ14" s="12"/>
       <c r="AR14" s="17"/>
       <c r="AS14" s="17"/>
-      <c r="AU14" s="19" t="s">
+      <c r="AU14" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="AV14" s="19"/>
-      <c r="AW14" s="19"/>
-      <c r="AX14" s="19"/>
-      <c r="AY14" s="19"/>
-      <c r="AZ14" s="19"/>
-      <c r="BA14" s="19"/>
+      <c r="AV14" s="43"/>
+      <c r="AW14" s="43"/>
+      <c r="AX14" s="43"/>
+      <c r="AY14" s="43"/>
+      <c r="AZ14" s="43"/>
+      <c r="BA14" s="43"/>
     </row>
     <row r="15" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1611,7 +1969,9 @@
       <c r="A16" s="7">
         <v>1</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="30">
+        <v>45402</v>
+      </c>
       <c r="C16" s="10" t="s">
         <v>8</v>
       </c>
@@ -1630,8 +1990,12 @@
       <c r="AU16" s="7">
         <v>1</v>
       </c>
-      <c r="AV16" s="49"/>
-      <c r="AW16" s="10"/>
+      <c r="AV16" s="30">
+        <v>45404</v>
+      </c>
+      <c r="AW16" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="AX16" s="11"/>
       <c r="AY16" s="10" t="s">
         <v>7</v>
@@ -1643,7 +2007,9 @@
       <c r="A17" s="8">
         <v>2</v>
       </c>
-      <c r="B17" s="50"/>
+      <c r="B17" s="31">
+        <v>45404</v>
+      </c>
       <c r="C17" s="12" t="s">
         <v>8</v>
       </c>
@@ -1662,8 +2028,12 @@
       <c r="AU17" s="8">
         <v>2</v>
       </c>
-      <c r="AV17" s="50"/>
-      <c r="AW17" s="12"/>
+      <c r="AV17" s="31">
+        <v>45406</v>
+      </c>
+      <c r="AW17" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="AX17" s="13"/>
       <c r="AY17" s="12" t="s">
         <v>7</v>
@@ -1675,7 +2045,9 @@
       <c r="A18" s="8">
         <v>3</v>
       </c>
-      <c r="B18" s="50"/>
+      <c r="B18" s="31">
+        <v>45407</v>
+      </c>
       <c r="C18" s="12" t="s">
         <v>4</v>
       </c>
@@ -1695,12 +2067,16 @@
       <c r="AU18" s="8">
         <v>3</v>
       </c>
-      <c r="AV18" s="50"/>
+      <c r="AV18" s="31">
+        <v>45408</v>
+      </c>
       <c r="AW18" s="12" t="s">
         <v>7</v>
       </c>
       <c r="AX18" s="13"/>
-      <c r="AY18" s="12"/>
+      <c r="AY18" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="AZ18" s="13"/>
       <c r="BA18" s="16"/>
     </row>
@@ -1708,7 +2084,9 @@
       <c r="A19" s="8">
         <v>4</v>
       </c>
-      <c r="B19" s="50"/>
+      <c r="B19" s="31">
+        <v>45409</v>
+      </c>
       <c r="C19" s="12" t="s">
         <v>4</v>
       </c>
@@ -1718,24 +2096,28 @@
       </c>
       <c r="F19" s="13"/>
       <c r="G19" s="16"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
       <c r="L19" s="12"/>
       <c r="O19" s="12"/>
       <c r="AN19" s="12"/>
-      <c r="AQ19" s="24"/>
-      <c r="AR19" s="23"/>
-      <c r="AS19" s="23"/>
+      <c r="AQ19" s="53"/>
+      <c r="AR19" s="42"/>
+      <c r="AS19" s="42"/>
       <c r="AU19" s="8">
         <v>4</v>
       </c>
-      <c r="AV19" s="50"/>
+      <c r="AV19" s="31">
+        <v>45410</v>
+      </c>
       <c r="AW19" s="12" t="s">
         <v>7</v>
       </c>
       <c r="AX19" s="13"/>
-      <c r="AY19" s="12"/>
+      <c r="AY19" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="AZ19" s="13"/>
       <c r="BA19" s="16"/>
     </row>
@@ -1743,7 +2125,7 @@
       <c r="A20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="50"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="12" t="s">
         <v>8</v>
       </c>
@@ -1760,8 +2142,10 @@
       <c r="AU20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AV20" s="50"/>
-      <c r="AW20" s="12"/>
+      <c r="AV20" s="31"/>
+      <c r="AW20" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="AX20" s="13"/>
       <c r="AY20" s="12" t="s">
         <v>7</v>
@@ -1773,7 +2157,7 @@
       <c r="A21" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="50"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="12" t="s">
         <v>4</v>
       </c>
@@ -1788,12 +2172,14 @@
       <c r="AU21" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AV21" s="50"/>
+      <c r="AV21" s="31"/>
       <c r="AW21" s="12" t="s">
         <v>7</v>
       </c>
       <c r="AX21" s="13"/>
-      <c r="AY21" s="12"/>
+      <c r="AY21" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="AZ21" s="13"/>
       <c r="BA21" s="16"/>
     </row>
@@ -1801,7 +2187,7 @@
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="51"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="14" t="s">
         <v>8</v>
       </c>
@@ -1816,8 +2202,10 @@
       <c r="AU22" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AV22" s="51"/>
-      <c r="AW22" s="14"/>
+      <c r="AV22" s="32"/>
+      <c r="AW22" s="14" t="s">
+        <v>9</v>
+      </c>
       <c r="AX22" s="15"/>
       <c r="AY22" s="14" t="s">
         <v>7</v>
@@ -1826,112 +2214,112 @@
       <c r="BA22" s="6"/>
     </row>
     <row r="23" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
       <c r="O23" s="12"/>
       <c r="AN23" s="12"/>
-      <c r="AU23" s="19" t="s">
+      <c r="AU23" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AV23" s="19"/>
-      <c r="AW23" s="19"/>
-      <c r="AX23" s="19"/>
-      <c r="AY23" s="19"/>
-      <c r="AZ23" s="19"/>
-      <c r="BA23" s="19"/>
+      <c r="AV23" s="43"/>
+      <c r="AW23" s="43"/>
+      <c r="AX23" s="43"/>
+      <c r="AY23" s="43"/>
+      <c r="AZ23" s="43"/>
+      <c r="BA23" s="43"/>
     </row>
     <row r="24" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O24" s="12"/>
       <c r="AN24" s="12"/>
     </row>
     <row r="25" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
       <c r="O25" s="12"/>
       <c r="AN25" s="12"/>
-      <c r="AU25" s="19" t="s">
+      <c r="AU25" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="AV25" s="19"/>
-      <c r="AW25" s="19"/>
-      <c r="AX25" s="19"/>
-      <c r="AY25" s="19"/>
-      <c r="AZ25" s="19"/>
-      <c r="BA25" s="19"/>
+      <c r="AV25" s="43"/>
+      <c r="AW25" s="43"/>
+      <c r="AX25" s="43"/>
+      <c r="AY25" s="43"/>
+      <c r="AZ25" s="43"/>
+      <c r="BA25" s="43"/>
     </row>
     <row r="26" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E26" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="34" t="s">
+      <c r="F26" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="34" t="s">
+      <c r="G26" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="O26" s="24"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
-      <c r="AE26" s="23"/>
-      <c r="AF26" s="23"/>
-      <c r="AG26" s="23"/>
-      <c r="AH26" s="23"/>
-      <c r="AI26" s="23"/>
-      <c r="AJ26" s="23"/>
-      <c r="AK26" s="23"/>
-      <c r="AL26" s="23"/>
-      <c r="AM26" s="25"/>
-      <c r="AU26" s="34" t="s">
+      <c r="O26" s="53"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="42"/>
+      <c r="S26" s="42"/>
+      <c r="T26" s="42"/>
+      <c r="U26" s="42"/>
+      <c r="V26" s="42"/>
+      <c r="W26" s="42"/>
+      <c r="AE26" s="42"/>
+      <c r="AF26" s="42"/>
+      <c r="AG26" s="42"/>
+      <c r="AH26" s="42"/>
+      <c r="AI26" s="42"/>
+      <c r="AJ26" s="42"/>
+      <c r="AK26" s="42"/>
+      <c r="AL26" s="42"/>
+      <c r="AM26" s="57"/>
+      <c r="AU26" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="AV26" s="34" t="s">
+      <c r="AV26" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="AW26" s="34" t="s">
+      <c r="AW26" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AX26" s="34" t="s">
+      <c r="AX26" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="AY26" s="34" t="s">
+      <c r="AY26" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="AZ26" s="34" t="s">
+      <c r="AZ26" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="BA26" s="34" t="s">
+      <c r="BA26" s="21" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1939,7 +2327,9 @@
       <c r="A27" s="7">
         <v>1</v>
       </c>
-      <c r="B27" s="49"/>
+      <c r="B27" s="30">
+        <v>45402</v>
+      </c>
       <c r="C27" s="10" t="s">
         <v>14</v>
       </c>
@@ -1961,7 +2351,9 @@
       <c r="AU27" s="7">
         <v>1</v>
       </c>
-      <c r="AV27" s="49"/>
+      <c r="AV27" s="30">
+        <v>45403</v>
+      </c>
       <c r="AW27" s="10" t="s">
         <v>3</v>
       </c>
@@ -1976,7 +2368,9 @@
       <c r="A28" s="8">
         <v>2</v>
       </c>
-      <c r="B28" s="50"/>
+      <c r="B28" s="31">
+        <v>45404</v>
+      </c>
       <c r="C28" s="12" t="s">
         <v>14</v>
       </c>
@@ -1987,15 +2381,15 @@
       <c r="F28" s="13"/>
       <c r="G28" s="16"/>
       <c r="O28" s="12"/>
-      <c r="P28" s="39" t="s">
+      <c r="P28" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="Q28" s="40"/>
-      <c r="R28" s="40"/>
-      <c r="S28" s="40"/>
-      <c r="T28" s="40"/>
-      <c r="U28" s="40"/>
-      <c r="V28" s="41"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="45"/>
+      <c r="S28" s="45"/>
+      <c r="T28" s="45"/>
+      <c r="U28" s="45"/>
+      <c r="V28" s="46"/>
       <c r="X28" s="12"/>
       <c r="Y28" s="17"/>
       <c r="Z28" s="17"/>
@@ -2003,20 +2397,22 @@
       <c r="AB28" s="17"/>
       <c r="AC28" s="17"/>
       <c r="AD28" s="13"/>
-      <c r="AF28" s="19" t="s">
+      <c r="AF28" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="AG28" s="19"/>
-      <c r="AH28" s="19"/>
-      <c r="AI28" s="19"/>
-      <c r="AJ28" s="19"/>
-      <c r="AK28" s="19"/>
-      <c r="AL28" s="19"/>
+      <c r="AG28" s="43"/>
+      <c r="AH28" s="43"/>
+      <c r="AI28" s="43"/>
+      <c r="AJ28" s="43"/>
+      <c r="AK28" s="43"/>
+      <c r="AL28" s="43"/>
       <c r="AN28" s="12"/>
       <c r="AU28" s="8">
         <v>2</v>
       </c>
-      <c r="AV28" s="50"/>
+      <c r="AV28" s="31">
+        <v>45405</v>
+      </c>
       <c r="AW28" s="12" t="s">
         <v>3</v>
       </c>
@@ -2031,7 +2427,9 @@
       <c r="A29" s="8">
         <v>3</v>
       </c>
-      <c r="B29" s="50"/>
+      <c r="B29" s="31">
+        <v>45406</v>
+      </c>
       <c r="C29" s="12" t="s">
         <v>2</v>
       </c>
@@ -2043,25 +2441,25 @@
       <c r="G29" s="16"/>
       <c r="I29" s="17"/>
       <c r="O29" s="12"/>
-      <c r="P29" s="38" t="s">
+      <c r="P29" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="Q29" s="38" t="s">
+      <c r="Q29" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="R29" s="38" t="s">
+      <c r="R29" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="S29" s="38" t="s">
+      <c r="S29" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="T29" s="38" t="s">
+      <c r="T29" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="U29" s="38" t="s">
+      <c r="U29" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="V29" s="38" t="s">
+      <c r="V29" s="25" t="s">
         <v>25</v>
       </c>
       <c r="X29" s="12"/>
@@ -2097,7 +2495,9 @@
       <c r="AU29" s="8">
         <v>3</v>
       </c>
-      <c r="AV29" s="50"/>
+      <c r="AV29" s="31">
+        <v>45408</v>
+      </c>
       <c r="AW29" s="12" t="s">
         <v>17</v>
       </c>
@@ -2112,7 +2512,9 @@
       <c r="A30" s="8">
         <v>4</v>
       </c>
-      <c r="B30" s="50"/>
+      <c r="B30" s="31">
+        <v>45409</v>
+      </c>
       <c r="C30" s="12" t="s">
         <v>2</v>
       </c>
@@ -2122,19 +2524,19 @@
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="16"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
       <c r="O30" s="12"/>
       <c r="P30" s="7">
         <v>1</v>
       </c>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="42"/>
-      <c r="S30" s="43"/>
-      <c r="T30" s="42"/>
-      <c r="U30" s="43"/>
-      <c r="V30" s="44"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="27"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="27"/>
+      <c r="V30" s="28"/>
       <c r="X30" s="12"/>
       <c r="Y30" s="17"/>
       <c r="Z30" s="17"/>
@@ -2145,20 +2547,22 @@
       <c r="AF30" s="7">
         <v>1</v>
       </c>
-      <c r="AG30" s="52"/>
-      <c r="AH30" s="42"/>
-      <c r="AI30" s="43"/>
-      <c r="AJ30" s="42"/>
-      <c r="AK30" s="43"/>
-      <c r="AL30" s="44"/>
+      <c r="AG30" s="33"/>
+      <c r="AH30" s="26"/>
+      <c r="AI30" s="27"/>
+      <c r="AJ30" s="26"/>
+      <c r="AK30" s="27"/>
+      <c r="AL30" s="28"/>
       <c r="AN30" s="12"/>
-      <c r="AQ30" s="23"/>
-      <c r="AR30" s="23"/>
-      <c r="AS30" s="23"/>
+      <c r="AQ30" s="42"/>
+      <c r="AR30" s="42"/>
+      <c r="AS30" s="42"/>
       <c r="AU30" s="8">
         <v>4</v>
       </c>
-      <c r="AV30" s="50"/>
+      <c r="AV30" s="31">
+        <v>45410</v>
+      </c>
       <c r="AW30" s="12" t="s">
         <v>17</v>
       </c>
@@ -2173,7 +2577,7 @@
       <c r="A31" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="50"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="12" t="s">
         <v>14</v>
       </c>
@@ -2189,7 +2593,7 @@
       <c r="P31" s="8">
         <v>2</v>
       </c>
-      <c r="Q31" s="37"/>
+      <c r="Q31" s="24"/>
       <c r="R31" s="12"/>
       <c r="S31" s="13"/>
       <c r="T31" s="12"/>
@@ -2205,7 +2609,7 @@
       <c r="AF31" s="8">
         <v>2</v>
       </c>
-      <c r="AG31" s="50"/>
+      <c r="AG31" s="31"/>
       <c r="AH31" s="12"/>
       <c r="AI31" s="13"/>
       <c r="AJ31" s="12"/>
@@ -2218,7 +2622,7 @@
       <c r="AU31" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AV31" s="50"/>
+      <c r="AV31" s="31"/>
       <c r="AW31" s="12" t="s">
         <v>3</v>
       </c>
@@ -2233,7 +2637,7 @@
       <c r="A32" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="50"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="12" t="s">
         <v>2</v>
       </c>
@@ -2248,7 +2652,7 @@
       <c r="P32" s="8">
         <v>3</v>
       </c>
-      <c r="Q32" s="37"/>
+      <c r="Q32" s="24"/>
       <c r="R32" s="12"/>
       <c r="S32" s="13"/>
       <c r="T32" s="12"/>
@@ -2264,7 +2668,7 @@
       <c r="AF32" s="8">
         <v>3</v>
       </c>
-      <c r="AG32" s="50"/>
+      <c r="AG32" s="31"/>
       <c r="AH32" s="12"/>
       <c r="AI32" s="13"/>
       <c r="AJ32" s="12"/>
@@ -2277,7 +2681,7 @@
       <c r="AU32" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AV32" s="50"/>
+      <c r="AV32" s="31"/>
       <c r="AW32" s="12" t="s">
         <v>17</v>
       </c>
@@ -2292,7 +2696,7 @@
       <c r="A33" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="51"/>
+      <c r="B33" s="32"/>
       <c r="C33" s="14" t="s">
         <v>14</v>
       </c>
@@ -2307,7 +2711,7 @@
       <c r="P33" s="8">
         <v>4</v>
       </c>
-      <c r="Q33" s="37"/>
+      <c r="Q33" s="24"/>
       <c r="R33" s="12"/>
       <c r="S33" s="13"/>
       <c r="T33" s="12"/>
@@ -2323,7 +2727,7 @@
       <c r="AF33" s="8">
         <v>4</v>
       </c>
-      <c r="AG33" s="56"/>
+      <c r="AG33" s="37"/>
       <c r="AH33" s="12"/>
       <c r="AI33" s="13"/>
       <c r="AJ33" s="12"/>
@@ -2336,7 +2740,7 @@
       <c r="AU33" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AV33" s="51"/>
+      <c r="AV33" s="32"/>
       <c r="AW33" s="14" t="s">
         <v>3</v>
       </c>
@@ -2348,21 +2752,21 @@
       <c r="BA33" s="6"/>
     </row>
     <row r="34" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
       <c r="L34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Q34" s="37"/>
+      <c r="Q34" s="24"/>
       <c r="R34" s="12"/>
       <c r="S34" s="13"/>
       <c r="T34" s="12"/>
@@ -2378,7 +2782,7 @@
       <c r="AF34" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AG34" s="50"/>
+      <c r="AG34" s="31"/>
       <c r="AH34" s="12"/>
       <c r="AI34" s="13"/>
       <c r="AJ34" s="12"/>
@@ -2388,15 +2792,15 @@
       <c r="AQ34" s="12"/>
       <c r="AR34" s="17"/>
       <c r="AS34" s="17"/>
-      <c r="AU34" s="19" t="s">
+      <c r="AU34" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AV34" s="19"/>
-      <c r="AW34" s="19"/>
-      <c r="AX34" s="19"/>
-      <c r="AY34" s="19"/>
-      <c r="AZ34" s="19"/>
-      <c r="BA34" s="19"/>
+      <c r="AV34" s="43"/>
+      <c r="AW34" s="43"/>
+      <c r="AX34" s="43"/>
+      <c r="AY34" s="43"/>
+      <c r="AZ34" s="43"/>
+      <c r="BA34" s="43"/>
     </row>
     <row r="35" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L35" s="12"/>
@@ -2404,7 +2808,7 @@
       <c r="P35" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="Q35" s="37"/>
+      <c r="Q35" s="24"/>
       <c r="R35" s="12"/>
       <c r="S35" s="13"/>
       <c r="T35" s="12"/>
@@ -2420,7 +2824,7 @@
       <c r="AF35" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AG35" s="50"/>
+      <c r="AG35" s="31"/>
       <c r="AH35" s="12"/>
       <c r="AI35" s="13"/>
       <c r="AJ35" s="12"/>
@@ -2432,23 +2836,23 @@
       <c r="AS35" s="17"/>
     </row>
     <row r="36" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="L36" s="24"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="23"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="L36" s="53"/>
+      <c r="M36" s="42"/>
+      <c r="N36" s="42"/>
       <c r="O36" s="12"/>
       <c r="P36" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q36" s="37"/>
+      <c r="Q36" s="24"/>
       <c r="R36" s="12"/>
       <c r="S36" s="13"/>
       <c r="T36" s="12"/>
@@ -2464,76 +2868,76 @@
       <c r="AF36" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AG36" s="57"/>
-      <c r="AH36" s="58"/>
-      <c r="AI36" s="59"/>
-      <c r="AJ36" s="58"/>
-      <c r="AK36" s="59"/>
-      <c r="AL36" s="60"/>
-      <c r="AN36" s="24"/>
-      <c r="AO36" s="23"/>
-      <c r="AP36" s="23"/>
+      <c r="AG36" s="38"/>
+      <c r="AH36" s="39"/>
+      <c r="AI36" s="40"/>
+      <c r="AJ36" s="39"/>
+      <c r="AK36" s="40"/>
+      <c r="AL36" s="41"/>
+      <c r="AN36" s="53"/>
+      <c r="AO36" s="42"/>
+      <c r="AP36" s="42"/>
       <c r="AQ36" s="12"/>
       <c r="AR36" s="17"/>
       <c r="AS36" s="17"/>
-      <c r="AU36" s="19" t="s">
+      <c r="AU36" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="AV36" s="19"/>
-      <c r="AW36" s="19"/>
-      <c r="AX36" s="19"/>
-      <c r="AY36" s="19"/>
-      <c r="AZ36" s="19"/>
-      <c r="BA36" s="19"/>
+      <c r="AV36" s="43"/>
+      <c r="AW36" s="43"/>
+      <c r="AX36" s="43"/>
+      <c r="AY36" s="43"/>
+      <c r="AZ36" s="43"/>
+      <c r="BA36" s="43"/>
     </row>
     <row r="37" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C37" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="34" t="s">
+      <c r="E37" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F37" s="34" t="s">
+      <c r="F37" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G37" s="34" t="s">
+      <c r="G37" s="21" t="s">
         <v>25</v>
       </c>
       <c r="L37" s="12"/>
-      <c r="P37" s="46" t="s">
+      <c r="P37" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Q37" s="47"/>
-      <c r="R37" s="47"/>
-      <c r="S37" s="47"/>
-      <c r="T37" s="47"/>
-      <c r="U37" s="47"/>
-      <c r="V37" s="48"/>
-      <c r="X37" s="24"/>
-      <c r="Y37" s="23"/>
-      <c r="Z37" s="23"/>
-      <c r="AA37" s="23"/>
-      <c r="AB37" s="23"/>
-      <c r="AC37" s="23"/>
-      <c r="AD37" s="25"/>
-      <c r="AF37" s="19" t="s">
+      <c r="Q37" s="48"/>
+      <c r="R37" s="48"/>
+      <c r="S37" s="48"/>
+      <c r="T37" s="48"/>
+      <c r="U37" s="48"/>
+      <c r="V37" s="49"/>
+      <c r="X37" s="53"/>
+      <c r="Y37" s="42"/>
+      <c r="Z37" s="42"/>
+      <c r="AA37" s="42"/>
+      <c r="AB37" s="42"/>
+      <c r="AC37" s="42"/>
+      <c r="AD37" s="57"/>
+      <c r="AF37" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AG37" s="19"/>
-      <c r="AH37" s="19"/>
-      <c r="AI37" s="19"/>
-      <c r="AJ37" s="19"/>
-      <c r="AK37" s="19"/>
-      <c r="AL37" s="19"/>
+      <c r="AG37" s="43"/>
+      <c r="AH37" s="43"/>
+      <c r="AI37" s="43"/>
+      <c r="AJ37" s="43"/>
+      <c r="AK37" s="43"/>
+      <c r="AL37" s="43"/>
       <c r="AQ37" s="12"/>
       <c r="AR37" s="17"/>
       <c r="AS37" s="17"/>
@@ -2563,7 +2967,9 @@
       <c r="A38" s="7">
         <v>1</v>
       </c>
-      <c r="B38" s="49"/>
+      <c r="B38" s="30">
+        <v>45403</v>
+      </c>
       <c r="C38" s="10" t="s">
         <v>12</v>
       </c>
@@ -2580,8 +2986,12 @@
       <c r="AU38" s="7">
         <v>1</v>
       </c>
-      <c r="AV38" s="49"/>
-      <c r="AW38" s="10"/>
+      <c r="AV38" s="30">
+        <v>45404</v>
+      </c>
+      <c r="AW38" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="AX38" s="11"/>
       <c r="AY38" s="10" t="s">
         <v>5</v>
@@ -2593,7 +3003,9 @@
       <c r="A39" s="8">
         <v>2</v>
       </c>
-      <c r="B39" s="50"/>
+      <c r="B39" s="31">
+        <v>45405</v>
+      </c>
       <c r="C39" s="12" t="s">
         <v>12</v>
       </c>
@@ -2604,41 +3016,45 @@
       <c r="F39" s="13"/>
       <c r="G39" s="16"/>
       <c r="L39" s="12"/>
-      <c r="M39" s="39" t="s">
+      <c r="M39" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="N39" s="40"/>
-      <c r="O39" s="40"/>
-      <c r="P39" s="40"/>
-      <c r="Q39" s="40"/>
-      <c r="R39" s="40"/>
-      <c r="S39" s="41"/>
-      <c r="X39" s="19" t="s">
+      <c r="N39" s="45"/>
+      <c r="O39" s="45"/>
+      <c r="P39" s="45"/>
+      <c r="Q39" s="45"/>
+      <c r="R39" s="45"/>
+      <c r="S39" s="46"/>
+      <c r="X39" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="Y39" s="19"/>
-      <c r="Z39" s="19"/>
-      <c r="AA39" s="19"/>
-      <c r="AB39" s="19"/>
-      <c r="AC39" s="19"/>
-      <c r="AD39" s="19"/>
-      <c r="AI39" s="19" t="s">
+      <c r="Y39" s="43"/>
+      <c r="Z39" s="43"/>
+      <c r="AA39" s="43"/>
+      <c r="AB39" s="43"/>
+      <c r="AC39" s="43"/>
+      <c r="AD39" s="43"/>
+      <c r="AI39" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="AJ39" s="19"/>
-      <c r="AK39" s="19"/>
-      <c r="AL39" s="19"/>
-      <c r="AM39" s="19"/>
-      <c r="AN39" s="19"/>
-      <c r="AO39" s="19"/>
+      <c r="AJ39" s="43"/>
+      <c r="AK39" s="43"/>
+      <c r="AL39" s="43"/>
+      <c r="AM39" s="43"/>
+      <c r="AN39" s="43"/>
+      <c r="AO39" s="43"/>
       <c r="AQ39" s="12"/>
       <c r="AR39" s="17"/>
       <c r="AS39" s="17"/>
       <c r="AU39" s="8">
         <v>2</v>
       </c>
-      <c r="AV39" s="50"/>
-      <c r="AW39" s="12"/>
+      <c r="AV39" s="31">
+        <v>45406</v>
+      </c>
+      <c r="AW39" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="AX39" s="13"/>
       <c r="AY39" s="12" t="s">
         <v>5</v>
@@ -2650,7 +3066,9 @@
       <c r="A40" s="8">
         <v>3</v>
       </c>
-      <c r="B40" s="50"/>
+      <c r="B40" s="31">
+        <v>45407</v>
+      </c>
       <c r="C40" s="12" t="s">
         <v>6</v>
       </c>
@@ -2662,25 +3080,25 @@
       <c r="G40" s="16"/>
       <c r="I40" s="17"/>
       <c r="L40" s="12"/>
-      <c r="M40" s="38" t="s">
+      <c r="M40" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="N40" s="38" t="s">
+      <c r="N40" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="O40" s="38" t="s">
+      <c r="O40" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="P40" s="38" t="s">
+      <c r="P40" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="Q40" s="38" t="s">
+      <c r="Q40" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="R40" s="38" t="s">
+      <c r="R40" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="S40" s="38" t="s">
+      <c r="S40" s="25" t="s">
         <v>25</v>
       </c>
       <c r="X40" s="3" t="s">
@@ -2731,12 +3149,16 @@
       <c r="AU40" s="8">
         <v>3</v>
       </c>
-      <c r="AV40" s="50"/>
+      <c r="AV40" s="31">
+        <v>45409</v>
+      </c>
       <c r="AW40" s="12" t="s">
         <v>5</v>
       </c>
       <c r="AX40" s="13"/>
-      <c r="AY40" s="12"/>
+      <c r="AY40" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="AZ40" s="13"/>
       <c r="BA40" s="16"/>
     </row>
@@ -2744,7 +3166,9 @@
       <c r="A41" s="8">
         <v>4</v>
       </c>
-      <c r="B41" s="50"/>
+      <c r="B41" s="31">
+        <v>45409</v>
+      </c>
       <c r="C41" s="12" t="s">
         <v>6</v>
       </c>
@@ -2754,49 +3178,53 @@
       </c>
       <c r="F41" s="13"/>
       <c r="G41" s="16"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="23"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="42"/>
+      <c r="K41" s="42"/>
       <c r="L41" s="12"/>
       <c r="M41" s="7">
         <v>1</v>
       </c>
-      <c r="N41" s="45"/>
-      <c r="O41" s="42"/>
-      <c r="P41" s="43"/>
-      <c r="Q41" s="42"/>
-      <c r="R41" s="43"/>
-      <c r="S41" s="44"/>
+      <c r="N41" s="29"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="27"/>
+      <c r="S41" s="28"/>
       <c r="X41" s="7">
         <v>1</v>
       </c>
-      <c r="Y41" s="52"/>
-      <c r="Z41" s="42"/>
-      <c r="AA41" s="43"/>
-      <c r="AB41" s="42"/>
-      <c r="AC41" s="43"/>
-      <c r="AD41" s="44"/>
+      <c r="Y41" s="33"/>
+      <c r="Z41" s="26"/>
+      <c r="AA41" s="27"/>
+      <c r="AB41" s="26"/>
+      <c r="AC41" s="27"/>
+      <c r="AD41" s="28"/>
       <c r="AI41" s="7">
         <v>1</v>
       </c>
-      <c r="AJ41" s="49"/>
+      <c r="AJ41" s="30"/>
       <c r="AK41" s="10"/>
       <c r="AL41" s="11"/>
       <c r="AM41" s="10"/>
       <c r="AN41" s="11"/>
       <c r="AO41" s="5"/>
-      <c r="AQ41" s="24"/>
-      <c r="AR41" s="23"/>
-      <c r="AS41" s="23"/>
+      <c r="AQ41" s="53"/>
+      <c r="AR41" s="42"/>
+      <c r="AS41" s="42"/>
       <c r="AU41" s="8">
         <v>4</v>
       </c>
-      <c r="AV41" s="50"/>
+      <c r="AV41" s="31">
+        <v>45411</v>
+      </c>
       <c r="AW41" s="12" t="s">
         <v>5</v>
       </c>
       <c r="AX41" s="13"/>
-      <c r="AY41" s="12"/>
+      <c r="AY41" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="AZ41" s="13"/>
       <c r="BA41" s="16"/>
     </row>
@@ -2804,7 +3232,7 @@
       <c r="A42" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="50"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="12" t="s">
         <v>12</v>
       </c>
@@ -2818,7 +3246,7 @@
       <c r="M42" s="8">
         <v>2</v>
       </c>
-      <c r="N42" s="37"/>
+      <c r="N42" s="24"/>
       <c r="O42" s="12"/>
       <c r="P42" s="13"/>
       <c r="Q42" s="12"/>
@@ -2827,7 +3255,7 @@
       <c r="X42" s="8">
         <v>2</v>
       </c>
-      <c r="Y42" s="50"/>
+      <c r="Y42" s="31"/>
       <c r="Z42" s="12"/>
       <c r="AA42" s="13"/>
       <c r="AB42" s="12"/>
@@ -2836,7 +3264,7 @@
       <c r="AI42" s="8">
         <v>2</v>
       </c>
-      <c r="AJ42" s="50"/>
+      <c r="AJ42" s="31"/>
       <c r="AK42" s="12"/>
       <c r="AL42" s="13"/>
       <c r="AM42" s="12"/>
@@ -2845,8 +3273,10 @@
       <c r="AU42" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AV42" s="50"/>
-      <c r="AW42" s="12"/>
+      <c r="AV42" s="31"/>
+      <c r="AW42" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="AX42" s="13"/>
       <c r="AY42" s="12" t="s">
         <v>5</v>
@@ -2858,7 +3288,7 @@
       <c r="A43" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B43" s="50"/>
+      <c r="B43" s="31"/>
       <c r="C43" s="12" t="s">
         <v>6</v>
       </c>
@@ -2871,7 +3301,7 @@
       <c r="M43" s="8">
         <v>3</v>
       </c>
-      <c r="N43" s="37"/>
+      <c r="N43" s="24"/>
       <c r="O43" s="12"/>
       <c r="P43" s="13"/>
       <c r="Q43" s="12"/>
@@ -2880,7 +3310,7 @@
       <c r="X43" s="8">
         <v>3</v>
       </c>
-      <c r="Y43" s="50"/>
+      <c r="Y43" s="31"/>
       <c r="Z43" s="12"/>
       <c r="AA43" s="13"/>
       <c r="AB43" s="12"/>
@@ -2889,7 +3319,7 @@
       <c r="AI43" s="8">
         <v>3</v>
       </c>
-      <c r="AJ43" s="50"/>
+      <c r="AJ43" s="31"/>
       <c r="AK43" s="12"/>
       <c r="AL43" s="13"/>
       <c r="AM43" s="12"/>
@@ -2898,10 +3328,14 @@
       <c r="AU43" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AV43" s="50"/>
-      <c r="AW43" s="12"/>
+      <c r="AV43" s="31"/>
+      <c r="AW43" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="AX43" s="13"/>
-      <c r="AY43" s="12"/>
+      <c r="AY43" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="AZ43" s="13"/>
       <c r="BA43" s="16"/>
     </row>
@@ -2909,7 +3343,7 @@
       <c r="A44" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="51"/>
+      <c r="B44" s="32"/>
       <c r="C44" s="14" t="s">
         <v>12</v>
       </c>
@@ -2922,7 +3356,7 @@
       <c r="M44" s="8">
         <v>4</v>
       </c>
-      <c r="N44" s="37"/>
+      <c r="N44" s="24"/>
       <c r="O44" s="12"/>
       <c r="P44" s="13"/>
       <c r="Q44" s="12"/>
@@ -2931,7 +3365,7 @@
       <c r="X44" s="8">
         <v>4</v>
       </c>
-      <c r="Y44" s="50"/>
+      <c r="Y44" s="31"/>
       <c r="Z44" s="12"/>
       <c r="AA44" s="13"/>
       <c r="AB44" s="12"/>
@@ -2940,7 +3374,7 @@
       <c r="AI44" s="8">
         <v>4</v>
       </c>
-      <c r="AJ44" s="56"/>
+      <c r="AJ44" s="37"/>
       <c r="AK44" s="12"/>
       <c r="AL44" s="13"/>
       <c r="AM44" s="12"/>
@@ -2949,8 +3383,10 @@
       <c r="AU44" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AV44" s="51"/>
-      <c r="AW44" s="14"/>
+      <c r="AV44" s="32"/>
+      <c r="AW44" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="AX44" s="15"/>
       <c r="AY44" s="14" t="s">
         <v>5</v>
@@ -2959,19 +3395,19 @@
       <c r="BA44" s="6"/>
     </row>
     <row r="45" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
       <c r="M45" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N45" s="37"/>
+      <c r="N45" s="24"/>
       <c r="O45" s="12"/>
       <c r="P45" s="13"/>
       <c r="Q45" s="12"/>
@@ -2980,7 +3416,7 @@
       <c r="X45" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Y45" s="50"/>
+      <c r="Y45" s="31"/>
       <c r="Z45" s="12"/>
       <c r="AA45" s="13"/>
       <c r="AB45" s="12"/>
@@ -2989,27 +3425,27 @@
       <c r="AI45" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AJ45" s="50"/>
+      <c r="AJ45" s="31"/>
       <c r="AK45" s="12"/>
       <c r="AL45" s="13"/>
       <c r="AM45" s="12"/>
       <c r="AN45" s="13"/>
       <c r="AO45" s="16"/>
-      <c r="AU45" s="19" t="s">
+      <c r="AU45" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AV45" s="19"/>
-      <c r="AW45" s="19"/>
-      <c r="AX45" s="19"/>
-      <c r="AY45" s="19"/>
-      <c r="AZ45" s="19"/>
-      <c r="BA45" s="19"/>
+      <c r="AV45" s="43"/>
+      <c r="AW45" s="43"/>
+      <c r="AX45" s="43"/>
+      <c r="AY45" s="43"/>
+      <c r="AZ45" s="43"/>
+      <c r="BA45" s="43"/>
     </row>
     <row r="46" spans="1:53" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="M46" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N46" s="37"/>
+      <c r="N46" s="24"/>
       <c r="O46" s="12"/>
       <c r="P46" s="13"/>
       <c r="Q46" s="12"/>
@@ -3018,7 +3454,7 @@
       <c r="X46" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="Y46" s="50"/>
+      <c r="Y46" s="31"/>
       <c r="Z46" s="12"/>
       <c r="AA46" s="13"/>
       <c r="AB46" s="12"/>
@@ -3027,7 +3463,7 @@
       <c r="AI46" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AJ46" s="50"/>
+      <c r="AJ46" s="31"/>
       <c r="AK46" s="12"/>
       <c r="AL46" s="13"/>
       <c r="AM46" s="12"/>
@@ -3038,7 +3474,7 @@
       <c r="M47" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="N47" s="37"/>
+      <c r="N47" s="24"/>
       <c r="O47" s="12"/>
       <c r="P47" s="13"/>
       <c r="Q47" s="12"/>
@@ -3047,7 +3483,7 @@
       <c r="X47" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="Y47" s="51"/>
+      <c r="Y47" s="32"/>
       <c r="Z47" s="14"/>
       <c r="AA47" s="15"/>
       <c r="AB47" s="14"/>
@@ -3056,7 +3492,7 @@
       <c r="AI47" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AJ47" s="51"/>
+      <c r="AJ47" s="32"/>
       <c r="AK47" s="14"/>
       <c r="AL47" s="15"/>
       <c r="AM47" s="14"/>
@@ -3064,61 +3500,49 @@
       <c r="AO47" s="6"/>
     </row>
     <row r="48" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M48" s="39" t="s">
+      <c r="M48" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="N48" s="40"/>
-      <c r="O48" s="40"/>
-      <c r="P48" s="40"/>
-      <c r="Q48" s="40"/>
-      <c r="R48" s="40"/>
-      <c r="S48" s="41"/>
-      <c r="X48" s="19" t="s">
+      <c r="N48" s="45"/>
+      <c r="O48" s="45"/>
+      <c r="P48" s="45"/>
+      <c r="Q48" s="45"/>
+      <c r="R48" s="45"/>
+      <c r="S48" s="46"/>
+      <c r="X48" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="Y48" s="19"/>
-      <c r="Z48" s="19"/>
-      <c r="AA48" s="19"/>
-      <c r="AB48" s="19"/>
-      <c r="AC48" s="19"/>
-      <c r="AD48" s="19"/>
-      <c r="AI48" s="19" t="s">
+      <c r="Y48" s="43"/>
+      <c r="Z48" s="43"/>
+      <c r="AA48" s="43"/>
+      <c r="AB48" s="43"/>
+      <c r="AC48" s="43"/>
+      <c r="AD48" s="43"/>
+      <c r="AI48" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AJ48" s="19"/>
-      <c r="AK48" s="19"/>
-      <c r="AL48" s="19"/>
-      <c r="AM48" s="19"/>
-      <c r="AN48" s="19"/>
-      <c r="AO48" s="19"/>
+      <c r="AJ48" s="43"/>
+      <c r="AK48" s="43"/>
+      <c r="AL48" s="43"/>
+      <c r="AM48" s="43"/>
+      <c r="AN48" s="43"/>
+      <c r="AO48" s="43"/>
     </row>
     <row r="49" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="M13:S13"/>
-    <mergeCell ref="M48:S48"/>
-    <mergeCell ref="M39:S39"/>
-    <mergeCell ref="P37:V37"/>
-    <mergeCell ref="P28:V28"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="O26:W26"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="M2:R2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="M4:S4"/>
+    <mergeCell ref="AU45:BA45"/>
+    <mergeCell ref="AF28:AL28"/>
+    <mergeCell ref="AF37:AL37"/>
+    <mergeCell ref="AQ30:AS30"/>
+    <mergeCell ref="AQ41:AS41"/>
+    <mergeCell ref="AU2:BA2"/>
+    <mergeCell ref="AU3:BA3"/>
+    <mergeCell ref="AU12:BA12"/>
+    <mergeCell ref="AU14:BA14"/>
+    <mergeCell ref="AU23:BA23"/>
+    <mergeCell ref="AU34:BA34"/>
+    <mergeCell ref="AU36:BA36"/>
     <mergeCell ref="X37:AD37"/>
     <mergeCell ref="AE26:AM26"/>
     <mergeCell ref="Z1:AB1"/>
@@ -3135,18 +3559,30 @@
     <mergeCell ref="AN36:AP36"/>
     <mergeCell ref="AQ8:AS8"/>
     <mergeCell ref="AQ19:AS19"/>
-    <mergeCell ref="AQ30:AS30"/>
-    <mergeCell ref="AQ41:AS41"/>
-    <mergeCell ref="AU2:BA2"/>
-    <mergeCell ref="AU3:BA3"/>
-    <mergeCell ref="AU12:BA12"/>
-    <mergeCell ref="AU14:BA14"/>
-    <mergeCell ref="AU23:BA23"/>
-    <mergeCell ref="AU34:BA34"/>
-    <mergeCell ref="AU36:BA36"/>
-    <mergeCell ref="AU45:BA45"/>
-    <mergeCell ref="AF28:AL28"/>
-    <mergeCell ref="AF37:AL37"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="O26:W26"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="L36:N36"/>
+    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="M4:S4"/>
+    <mergeCell ref="M13:S13"/>
+    <mergeCell ref="M48:S48"/>
+    <mergeCell ref="M39:S39"/>
+    <mergeCell ref="P37:V37"/>
+    <mergeCell ref="P28:V28"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A34:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3247,353 +3683,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="31"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="31"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="31"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L39" s="2"/>
-    </row>
-    <row r="40" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L41" s="2"/>
-    </row>
-    <row r="42" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L42" s="2"/>
-    </row>
-    <row r="43" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="H44" s="2"/>
-      <c r="L44" s="2"/>
-    </row>
-    <row r="45" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="H45" s="2"/>
-      <c r="L45" s="2"/>
-    </row>
-    <row r="46" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="L46" s="2"/>
-    </row>
-    <row r="48" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L48" s="2"/>
-    </row>
-    <row r="49" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="H49" s="2"/>
-      <c r="L49" s="2"/>
-    </row>
-    <row r="50" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L50" s="2"/>
-    </row>
-    <row r="51" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G51" s="2"/>
-      <c r="L51" s="2"/>
-    </row>
-    <row r="52" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="L52" s="2"/>
-    </row>
-    <row r="53" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G53" s="2"/>
-      <c r="L53" s="2"/>
-    </row>
-    <row r="54" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="L54" s="2"/>
-    </row>
-    <row r="55" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="L55" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A16:B16"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Box Scores, Brackets
First 2 games 4/22/24
</commit_message>
<xml_diff>
--- a/2024/Playoffs/Brackets.xlsx
+++ b/2024/Playoffs/Brackets.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LunchProjects\GitHub\NHLStats\2024\Playoffs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\NHLStats\2024\Playoffs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE60A59-5310-4EC2-A804-E156B2152CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matchups" sheetId="3" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="58">
   <si>
     <t>Eastern Conference Playoff Teams</t>
   </si>
@@ -193,12 +194,18 @@
   </si>
   <si>
     <t>Canucks Lead 1-0</t>
+  </si>
+  <si>
+    <t>Hurricanes Lead 2-0</t>
+  </si>
+  <si>
+    <t>Series Tied 1-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -568,13 +575,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -594,36 +631,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -904,7 +911,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -997,18 +1004,18 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43" t="s">
+      <c r="D11" s="41"/>
+      <c r="E11" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="43"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="4" t="s">
         <v>40</v>
       </c>
@@ -1037,18 +1044,18 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="41" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="41" t="s">
+      <c r="D13" s="43"/>
+      <c r="E13" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="42"/>
+      <c r="F13" s="43"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1077,14 +1084,14 @@
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="41" t="s">
+      <c r="B16" s="43"/>
+      <c r="C16" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="42"/>
+      <c r="D16" s="43"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1107,10 +1114,10 @@
       <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="42"/>
+      <c r="B19" s="43"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1129,10 +1136,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="42"/>
+      <c r="B22" s="43"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -1214,16 +1221,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1231,11 +1238,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BA49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AX6" sqref="AX6"/>
+    <sheetView tabSelected="1" topLeftCell="AD13" workbookViewId="0">
+      <selection activeCell="AX38" sqref="AX38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,124 +1287,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="54"/>
-      <c r="Z1" s="52" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="53"/>
+      <c r="Z1" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="54"/>
-      <c r="AF1" s="52" t="s">
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="53"/>
+      <c r="AF1" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
-      <c r="AW1" s="53"/>
-      <c r="AX1" s="53"/>
-      <c r="AY1" s="53"/>
-      <c r="AZ1" s="53"/>
-      <c r="BA1" s="54"/>
+      <c r="AG1" s="52"/>
+      <c r="AH1" s="52"/>
+      <c r="AI1" s="52"/>
+      <c r="AJ1" s="52"/>
+      <c r="AK1" s="52"/>
+      <c r="AL1" s="52"/>
+      <c r="AM1" s="52"/>
+      <c r="AN1" s="52"/>
+      <c r="AO1" s="52"/>
+      <c r="AP1" s="52"/>
+      <c r="AQ1" s="52"/>
+      <c r="AR1" s="52"/>
+      <c r="AS1" s="52"/>
+      <c r="AT1" s="52"/>
+      <c r="AU1" s="52"/>
+      <c r="AV1" s="52"/>
+      <c r="AW1" s="52"/>
+      <c r="AX1" s="52"/>
+      <c r="AY1" s="52"/>
+      <c r="AZ1" s="52"/>
+      <c r="BA1" s="53"/>
     </row>
     <row r="2" spans="1:53" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="M2" s="56" t="s">
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="49"/>
+      <c r="M2" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="58"/>
-      <c r="AI2" s="56" t="s">
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="49"/>
+      <c r="AI2" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="AJ2" s="57"/>
-      <c r="AK2" s="57"/>
-      <c r="AL2" s="57"/>
-      <c r="AM2" s="57"/>
-      <c r="AN2" s="57"/>
-      <c r="AO2" s="58"/>
-      <c r="AU2" s="56" t="s">
+      <c r="AJ2" s="48"/>
+      <c r="AK2" s="48"/>
+      <c r="AL2" s="48"/>
+      <c r="AM2" s="48"/>
+      <c r="AN2" s="48"/>
+      <c r="AO2" s="49"/>
+      <c r="AU2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="AV2" s="57"/>
-      <c r="AW2" s="57"/>
-      <c r="AX2" s="57"/>
-      <c r="AY2" s="57"/>
-      <c r="AZ2" s="57"/>
-      <c r="BA2" s="58"/>
+      <c r="AV2" s="48"/>
+      <c r="AW2" s="48"/>
+      <c r="AX2" s="48"/>
+      <c r="AY2" s="48"/>
+      <c r="AZ2" s="48"/>
+      <c r="BA2" s="49"/>
     </row>
     <row r="3" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="AI3" s="50" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="AI3" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="AJ3" s="50"/>
-      <c r="AK3" s="50"/>
-      <c r="AL3" s="50"/>
-      <c r="AM3" s="50"/>
-      <c r="AN3" s="50"/>
-      <c r="AO3" s="50"/>
-      <c r="AU3" s="50" t="s">
+      <c r="AJ3" s="44"/>
+      <c r="AK3" s="44"/>
+      <c r="AL3" s="44"/>
+      <c r="AM3" s="44"/>
+      <c r="AN3" s="44"/>
+      <c r="AO3" s="44"/>
+      <c r="AU3" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="AV3" s="50"/>
-      <c r="AW3" s="50"/>
-      <c r="AX3" s="50"/>
-      <c r="AY3" s="50"/>
-      <c r="AZ3" s="50"/>
-      <c r="BA3" s="50"/>
+      <c r="AV3" s="44"/>
+      <c r="AW3" s="44"/>
+      <c r="AX3" s="44"/>
+      <c r="AY3" s="44"/>
+      <c r="AZ3" s="44"/>
+      <c r="BA3" s="44"/>
     </row>
     <row r="4" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -1421,15 +1428,15 @@
       <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="44" t="s">
+      <c r="M4" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="46"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="55"/>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="55"/>
+      <c r="S4" s="56"/>
       <c r="AI4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1657,9 +1664,9 @@
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="16"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
       <c r="M8" s="8">
         <v>3</v>
       </c>
@@ -1678,9 +1685,9 @@
       <c r="AM8" s="33"/>
       <c r="AN8" s="34"/>
       <c r="AO8" s="35"/>
-      <c r="AQ8" s="51"/>
-      <c r="AR8" s="51"/>
-      <c r="AS8" s="51"/>
+      <c r="AQ8" s="45"/>
+      <c r="AR8" s="45"/>
+      <c r="AS8" s="45"/>
       <c r="AU8" s="8">
         <v>4</v>
       </c>
@@ -1844,15 +1851,15 @@
       <c r="BA11" s="6"/>
     </row>
     <row r="12" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
       <c r="L12" s="12"/>
       <c r="M12" s="8" t="s">
         <v>28</v>
@@ -1863,65 +1870,65 @@
       <c r="Q12" s="12"/>
       <c r="R12" s="13"/>
       <c r="S12" s="16"/>
-      <c r="AI12" s="50" t="s">
+      <c r="AI12" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="AJ12" s="50"/>
-      <c r="AK12" s="50"/>
-      <c r="AL12" s="50"/>
-      <c r="AM12" s="50"/>
-      <c r="AN12" s="50"/>
-      <c r="AO12" s="50"/>
+      <c r="AJ12" s="44"/>
+      <c r="AK12" s="44"/>
+      <c r="AL12" s="44"/>
+      <c r="AM12" s="44"/>
+      <c r="AN12" s="44"/>
+      <c r="AO12" s="44"/>
       <c r="AQ12" s="12"/>
-      <c r="AU12" s="50" t="s">
+      <c r="AU12" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="AV12" s="50"/>
-      <c r="AW12" s="50"/>
-      <c r="AX12" s="50"/>
-      <c r="AY12" s="50"/>
-      <c r="AZ12" s="50"/>
-      <c r="BA12" s="50"/>
+      <c r="AV12" s="44"/>
+      <c r="AW12" s="44"/>
+      <c r="AX12" s="44"/>
+      <c r="AY12" s="44"/>
+      <c r="AZ12" s="44"/>
+      <c r="BA12" s="44"/>
     </row>
     <row r="13" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L13" s="12"/>
-      <c r="M13" s="44" t="s">
+      <c r="M13" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="45"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="46"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="55"/>
+      <c r="R13" s="55"/>
+      <c r="S13" s="56"/>
       <c r="AQ13" s="12"/>
     </row>
     <row r="14" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
-      <c r="AN14" s="51"/>
-      <c r="AO14" s="51"/>
-      <c r="AP14" s="51"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="45"/>
+      <c r="AN14" s="45"/>
+      <c r="AO14" s="45"/>
+      <c r="AP14" s="45"/>
       <c r="AQ14" s="12"/>
-      <c r="AU14" s="50" t="s">
+      <c r="AU14" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="AV14" s="50"/>
-      <c r="AW14" s="50"/>
-      <c r="AX14" s="50"/>
-      <c r="AY14" s="50"/>
-      <c r="AZ14" s="50"/>
-      <c r="BA14" s="50"/>
+      <c r="AV14" s="44"/>
+      <c r="AW14" s="44"/>
+      <c r="AX14" s="44"/>
+      <c r="AY14" s="44"/>
+      <c r="AZ14" s="44"/>
+      <c r="BA14" s="44"/>
     </row>
     <row r="15" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -2023,12 +2030,18 @@
       <c r="C17" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="13">
+        <v>3</v>
+      </c>
       <c r="E17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="16"/>
+      <c r="F17" s="13">
+        <v>5</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>56</v>
+      </c>
       <c r="L17" s="12"/>
       <c r="O17" s="12"/>
       <c r="AN17" s="12"/>
@@ -2101,15 +2114,15 @@
       </c>
       <c r="F19" s="13"/>
       <c r="G19" s="16"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
       <c r="L19" s="12"/>
       <c r="O19" s="12"/>
       <c r="AN19" s="12"/>
-      <c r="AQ19" s="55"/>
-      <c r="AR19" s="51"/>
-      <c r="AS19" s="51"/>
+      <c r="AQ19" s="46"/>
+      <c r="AR19" s="45"/>
+      <c r="AS19" s="45"/>
       <c r="AU19" s="8">
         <v>4</v>
       </c>
@@ -2217,52 +2230,52 @@
       <c r="BA22" s="6"/>
     </row>
     <row r="23" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
       <c r="O23" s="12"/>
       <c r="AN23" s="12"/>
-      <c r="AU23" s="50" t="s">
+      <c r="AU23" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="AV23" s="50"/>
-      <c r="AW23" s="50"/>
-      <c r="AX23" s="50"/>
-      <c r="AY23" s="50"/>
-      <c r="AZ23" s="50"/>
-      <c r="BA23" s="50"/>
+      <c r="AV23" s="44"/>
+      <c r="AW23" s="44"/>
+      <c r="AX23" s="44"/>
+      <c r="AY23" s="44"/>
+      <c r="AZ23" s="44"/>
+      <c r="BA23" s="44"/>
     </row>
     <row r="24" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O24" s="12"/>
       <c r="AN24" s="12"/>
     </row>
     <row r="25" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
       <c r="O25" s="12"/>
       <c r="AN25" s="12"/>
-      <c r="AU25" s="50" t="s">
+      <c r="AU25" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="AV25" s="50"/>
-      <c r="AW25" s="50"/>
-      <c r="AX25" s="50"/>
-      <c r="AY25" s="50"/>
-      <c r="AZ25" s="50"/>
-      <c r="BA25" s="50"/>
+      <c r="AV25" s="44"/>
+      <c r="AW25" s="44"/>
+      <c r="AX25" s="44"/>
+      <c r="AY25" s="44"/>
+      <c r="AZ25" s="44"/>
+      <c r="BA25" s="44"/>
     </row>
     <row r="26" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="20" t="s">
@@ -2286,24 +2299,24 @@
       <c r="G26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="O26" s="55"/>
-      <c r="P26" s="51"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="51"/>
-      <c r="T26" s="51"/>
-      <c r="U26" s="51"/>
-      <c r="V26" s="51"/>
-      <c r="W26" s="51"/>
-      <c r="AE26" s="51"/>
-      <c r="AF26" s="51"/>
-      <c r="AG26" s="51"/>
-      <c r="AH26" s="51"/>
-      <c r="AI26" s="51"/>
-      <c r="AJ26" s="51"/>
-      <c r="AK26" s="51"/>
-      <c r="AL26" s="51"/>
-      <c r="AM26" s="59"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="45"/>
+      <c r="Q26" s="45"/>
+      <c r="R26" s="45"/>
+      <c r="S26" s="45"/>
+      <c r="T26" s="45"/>
+      <c r="U26" s="45"/>
+      <c r="V26" s="45"/>
+      <c r="W26" s="45"/>
+      <c r="AE26" s="45"/>
+      <c r="AF26" s="45"/>
+      <c r="AG26" s="45"/>
+      <c r="AH26" s="45"/>
+      <c r="AI26" s="45"/>
+      <c r="AJ26" s="45"/>
+      <c r="AK26" s="45"/>
+      <c r="AL26" s="45"/>
+      <c r="AM26" s="50"/>
       <c r="AU26" s="20" t="s">
         <v>18</v>
       </c>
@@ -2384,33 +2397,39 @@
       <c r="C28" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="13"/>
+      <c r="D28" s="13">
+        <v>3</v>
+      </c>
       <c r="E28" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="16"/>
+      <c r="F28" s="13">
+        <v>2</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>57</v>
+      </c>
       <c r="O28" s="12"/>
-      <c r="P28" s="44" t="s">
+      <c r="P28" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="45"/>
-      <c r="U28" s="45"/>
-      <c r="V28" s="46"/>
+      <c r="Q28" s="55"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="55"/>
+      <c r="T28" s="55"/>
+      <c r="U28" s="55"/>
+      <c r="V28" s="56"/>
       <c r="X28" s="12"/>
       <c r="AD28" s="13"/>
-      <c r="AF28" s="50" t="s">
+      <c r="AF28" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="AG28" s="50"/>
-      <c r="AH28" s="50"/>
-      <c r="AI28" s="50"/>
-      <c r="AJ28" s="50"/>
-      <c r="AK28" s="50"/>
-      <c r="AL28" s="50"/>
+      <c r="AG28" s="44"/>
+      <c r="AH28" s="44"/>
+      <c r="AI28" s="44"/>
+      <c r="AJ28" s="44"/>
+      <c r="AK28" s="44"/>
+      <c r="AL28" s="44"/>
       <c r="AN28" s="12"/>
       <c r="AU28" s="8">
         <v>2</v>
@@ -2522,9 +2541,9 @@
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="16"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
       <c r="O30" s="12"/>
       <c r="P30" s="7">
         <v>1</v>
@@ -2547,9 +2566,9 @@
       <c r="AK30" s="26"/>
       <c r="AL30" s="27"/>
       <c r="AN30" s="12"/>
-      <c r="AQ30" s="51"/>
-      <c r="AR30" s="51"/>
-      <c r="AS30" s="51"/>
+      <c r="AQ30" s="45"/>
+      <c r="AR30" s="45"/>
+      <c r="AS30" s="45"/>
       <c r="AU30" s="8">
         <v>4</v>
       </c>
@@ -2725,15 +2744,15 @@
       <c r="BA33" s="6"/>
     </row>
     <row r="34" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="50" t="s">
+      <c r="A34" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="50"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
       <c r="L34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="8" t="s">
@@ -2758,15 +2777,15 @@
       <c r="AL34" s="16"/>
       <c r="AN34" s="12"/>
       <c r="AQ34" s="12"/>
-      <c r="AU34" s="50" t="s">
+      <c r="AU34" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="AV34" s="50"/>
-      <c r="AW34" s="50"/>
-      <c r="AX34" s="50"/>
-      <c r="AY34" s="50"/>
-      <c r="AZ34" s="50"/>
-      <c r="BA34" s="50"/>
+      <c r="AV34" s="44"/>
+      <c r="AW34" s="44"/>
+      <c r="AX34" s="44"/>
+      <c r="AY34" s="44"/>
+      <c r="AZ34" s="44"/>
+      <c r="BA34" s="44"/>
     </row>
     <row r="35" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L35" s="12"/>
@@ -2795,18 +2814,18 @@
       <c r="AQ35" s="12"/>
     </row>
     <row r="36" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="51"/>
-      <c r="N36" s="51"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="45"/>
+      <c r="N36" s="45"/>
       <c r="O36" s="12"/>
       <c r="P36" s="8" t="s">
         <v>28</v>
@@ -2828,19 +2847,19 @@
       <c r="AJ36" s="38"/>
       <c r="AK36" s="39"/>
       <c r="AL36" s="40"/>
-      <c r="AN36" s="55"/>
-      <c r="AO36" s="51"/>
-      <c r="AP36" s="51"/>
+      <c r="AN36" s="46"/>
+      <c r="AO36" s="45"/>
+      <c r="AP36" s="45"/>
       <c r="AQ36" s="12"/>
-      <c r="AU36" s="50" t="s">
+      <c r="AU36" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="AV36" s="50"/>
-      <c r="AW36" s="50"/>
-      <c r="AX36" s="50"/>
-      <c r="AY36" s="50"/>
-      <c r="AZ36" s="50"/>
-      <c r="BA36" s="50"/>
+      <c r="AV36" s="44"/>
+      <c r="AW36" s="44"/>
+      <c r="AX36" s="44"/>
+      <c r="AY36" s="44"/>
+      <c r="AZ36" s="44"/>
+      <c r="BA36" s="44"/>
     </row>
     <row r="37" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="20" t="s">
@@ -2865,31 +2884,31 @@
         <v>25</v>
       </c>
       <c r="L37" s="12"/>
-      <c r="P37" s="47" t="s">
+      <c r="P37" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Q37" s="48"/>
-      <c r="R37" s="48"/>
-      <c r="S37" s="48"/>
-      <c r="T37" s="48"/>
-      <c r="U37" s="48"/>
-      <c r="V37" s="49"/>
-      <c r="X37" s="55"/>
-      <c r="Y37" s="51"/>
-      <c r="Z37" s="51"/>
-      <c r="AA37" s="51"/>
-      <c r="AB37" s="51"/>
-      <c r="AC37" s="51"/>
-      <c r="AD37" s="59"/>
-      <c r="AF37" s="50" t="s">
+      <c r="Q37" s="58"/>
+      <c r="R37" s="58"/>
+      <c r="S37" s="58"/>
+      <c r="T37" s="58"/>
+      <c r="U37" s="58"/>
+      <c r="V37" s="59"/>
+      <c r="X37" s="46"/>
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="45"/>
+      <c r="AA37" s="45"/>
+      <c r="AB37" s="45"/>
+      <c r="AC37" s="45"/>
+      <c r="AD37" s="50"/>
+      <c r="AF37" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="AG37" s="50"/>
-      <c r="AH37" s="50"/>
-      <c r="AI37" s="50"/>
-      <c r="AJ37" s="50"/>
-      <c r="AK37" s="50"/>
-      <c r="AL37" s="50"/>
+      <c r="AG37" s="44"/>
+      <c r="AH37" s="44"/>
+      <c r="AI37" s="44"/>
+      <c r="AJ37" s="44"/>
+      <c r="AK37" s="44"/>
+      <c r="AL37" s="44"/>
       <c r="AQ37" s="12"/>
       <c r="AU37" s="3" t="s">
         <v>18</v>
@@ -2970,33 +2989,33 @@
       <c r="F39" s="13"/>
       <c r="G39" s="16"/>
       <c r="L39" s="12"/>
-      <c r="M39" s="44" t="s">
+      <c r="M39" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
-      <c r="P39" s="45"/>
-      <c r="Q39" s="45"/>
-      <c r="R39" s="45"/>
-      <c r="S39" s="46"/>
-      <c r="X39" s="50" t="s">
+      <c r="N39" s="55"/>
+      <c r="O39" s="55"/>
+      <c r="P39" s="55"/>
+      <c r="Q39" s="55"/>
+      <c r="R39" s="55"/>
+      <c r="S39" s="56"/>
+      <c r="X39" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="Y39" s="50"/>
-      <c r="Z39" s="50"/>
-      <c r="AA39" s="50"/>
-      <c r="AB39" s="50"/>
-      <c r="AC39" s="50"/>
-      <c r="AD39" s="50"/>
-      <c r="AI39" s="50" t="s">
+      <c r="Y39" s="44"/>
+      <c r="Z39" s="44"/>
+      <c r="AA39" s="44"/>
+      <c r="AB39" s="44"/>
+      <c r="AC39" s="44"/>
+      <c r="AD39" s="44"/>
+      <c r="AI39" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="AJ39" s="50"/>
-      <c r="AK39" s="50"/>
-      <c r="AL39" s="50"/>
-      <c r="AM39" s="50"/>
-      <c r="AN39" s="50"/>
-      <c r="AO39" s="50"/>
+      <c r="AJ39" s="44"/>
+      <c r="AK39" s="44"/>
+      <c r="AL39" s="44"/>
+      <c r="AM39" s="44"/>
+      <c r="AN39" s="44"/>
+      <c r="AO39" s="44"/>
       <c r="AQ39" s="12"/>
       <c r="AU39" s="8">
         <v>2</v>
@@ -3127,9 +3146,9 @@
       </c>
       <c r="F41" s="13"/>
       <c r="G41" s="16"/>
-      <c r="I41" s="51"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="51"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="45"/>
+      <c r="K41" s="45"/>
       <c r="L41" s="12"/>
       <c r="M41" s="7">
         <v>1</v>
@@ -3158,9 +3177,9 @@
       <c r="AM41" s="10"/>
       <c r="AN41" s="11"/>
       <c r="AO41" s="5"/>
-      <c r="AQ41" s="55"/>
-      <c r="AR41" s="51"/>
-      <c r="AS41" s="51"/>
+      <c r="AQ41" s="46"/>
+      <c r="AR41" s="45"/>
+      <c r="AS41" s="45"/>
       <c r="AU41" s="8">
         <v>4</v>
       </c>
@@ -3343,15 +3362,15 @@
       <c r="BA44" s="6"/>
     </row>
     <row r="45" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="50" t="s">
+      <c r="A45" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="44"/>
       <c r="M45" s="8" t="s">
         <v>27</v>
       </c>
@@ -3379,15 +3398,15 @@
       <c r="AM45" s="12"/>
       <c r="AN45" s="13"/>
       <c r="AO45" s="16"/>
-      <c r="AU45" s="50" t="s">
+      <c r="AU45" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="AV45" s="50"/>
-      <c r="AW45" s="50"/>
-      <c r="AX45" s="50"/>
-      <c r="AY45" s="50"/>
-      <c r="AZ45" s="50"/>
-      <c r="BA45" s="50"/>
+      <c r="AV45" s="44"/>
+      <c r="AW45" s="44"/>
+      <c r="AX45" s="44"/>
+      <c r="AY45" s="44"/>
+      <c r="AZ45" s="44"/>
+      <c r="BA45" s="44"/>
     </row>
     <row r="46" spans="1:53" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="M46" s="8" t="s">
@@ -3448,49 +3467,61 @@
       <c r="AO47" s="6"/>
     </row>
     <row r="48" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M48" s="44" t="s">
+      <c r="M48" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="N48" s="45"/>
-      <c r="O48" s="45"/>
-      <c r="P48" s="45"/>
-      <c r="Q48" s="45"/>
-      <c r="R48" s="45"/>
-      <c r="S48" s="46"/>
-      <c r="X48" s="50" t="s">
+      <c r="N48" s="55"/>
+      <c r="O48" s="55"/>
+      <c r="P48" s="55"/>
+      <c r="Q48" s="55"/>
+      <c r="R48" s="55"/>
+      <c r="S48" s="56"/>
+      <c r="X48" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="Y48" s="50"/>
-      <c r="Z48" s="50"/>
-      <c r="AA48" s="50"/>
-      <c r="AB48" s="50"/>
-      <c r="AC48" s="50"/>
-      <c r="AD48" s="50"/>
-      <c r="AI48" s="50" t="s">
+      <c r="Y48" s="44"/>
+      <c r="Z48" s="44"/>
+      <c r="AA48" s="44"/>
+      <c r="AB48" s="44"/>
+      <c r="AC48" s="44"/>
+      <c r="AD48" s="44"/>
+      <c r="AI48" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="AJ48" s="50"/>
-      <c r="AK48" s="50"/>
-      <c r="AL48" s="50"/>
-      <c r="AM48" s="50"/>
-      <c r="AN48" s="50"/>
-      <c r="AO48" s="50"/>
+      <c r="AJ48" s="44"/>
+      <c r="AK48" s="44"/>
+      <c r="AL48" s="44"/>
+      <c r="AM48" s="44"/>
+      <c r="AN48" s="44"/>
+      <c r="AO48" s="44"/>
     </row>
     <row r="49" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="AU45:BA45"/>
-    <mergeCell ref="AF28:AL28"/>
-    <mergeCell ref="AF37:AL37"/>
-    <mergeCell ref="AQ30:AS30"/>
-    <mergeCell ref="AQ41:AS41"/>
-    <mergeCell ref="AU34:BA34"/>
-    <mergeCell ref="AU36:BA36"/>
-    <mergeCell ref="AU2:BA2"/>
-    <mergeCell ref="AU3:BA3"/>
-    <mergeCell ref="AU12:BA12"/>
-    <mergeCell ref="AU14:BA14"/>
-    <mergeCell ref="AU23:BA23"/>
+    <mergeCell ref="M48:S48"/>
+    <mergeCell ref="M39:S39"/>
+    <mergeCell ref="P37:V37"/>
+    <mergeCell ref="P28:V28"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="O26:W26"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="L36:N36"/>
+    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="M4:S4"/>
+    <mergeCell ref="M13:S13"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="A25:G25"/>
     <mergeCell ref="X37:AD37"/>
     <mergeCell ref="AE26:AM26"/>
     <mergeCell ref="Z1:AB1"/>
@@ -3507,121 +3538,109 @@
     <mergeCell ref="AN36:AP36"/>
     <mergeCell ref="AQ8:AS8"/>
     <mergeCell ref="AQ19:AS19"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="O26:W26"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="M2:R2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="M4:S4"/>
-    <mergeCell ref="M13:S13"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="M48:S48"/>
-    <mergeCell ref="M39:S39"/>
-    <mergeCell ref="P37:V37"/>
-    <mergeCell ref="P28:V28"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="AU2:BA2"/>
+    <mergeCell ref="AU3:BA3"/>
+    <mergeCell ref="AU12:BA12"/>
+    <mergeCell ref="AU14:BA14"/>
+    <mergeCell ref="AU23:BA23"/>
+    <mergeCell ref="AU45:BA45"/>
+    <mergeCell ref="AF28:AL28"/>
+    <mergeCell ref="AF37:AL37"/>
+    <mergeCell ref="AQ30:AS30"/>
+    <mergeCell ref="AQ41:AS41"/>
+    <mergeCell ref="AU34:BA34"/>
+    <mergeCell ref="AU36:BA36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="15">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$14:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C11 E5:E11 I8:K8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$20:$A$21</xm:f>
           </x14:formula1>
           <xm:sqref>C16:C22 E16:E22 I19:K19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$23:$A$24</xm:f>
           </x14:formula1>
           <xm:sqref>C27:C33 E27:E33 I30:K30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$17:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>C38:C44 E38:E44 I41:K41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>Matchups!$C$14:$C$15</xm:f>
           </x14:formula1>
           <xm:sqref>L14:N14 N6:O12 Q6:Q12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>Matchups!$C$17:$C$18</xm:f>
           </x14:formula1>
           <xm:sqref>L36:N36 N41:O47 Q41:Q47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>Matchups!$E$14:$E$15</xm:f>
           </x14:formula1>
           <xm:sqref>T30:T36 Q30:R36 O26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>Matchups!$F$14:$F$15</xm:f>
           </x14:formula1>
           <xm:sqref>AE26:AM26 AJ30:AJ36 AH30:AH36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>Matchups!$G$13:$G$14</xm:f>
           </x14:formula1>
           <xm:sqref>X37:AD37 Z41:Z47 AB41:AB47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$14:$B$15</xm:f>
           </x14:formula1>
           <xm:sqref>AW5:AW11 AY5:AY11 AQ8:AS8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$20:$B$21</xm:f>
           </x14:formula1>
           <xm:sqref>AW16:AW22 AY16:AY22 AQ19:AS19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$23:$B$24</xm:f>
           </x14:formula1>
           <xm:sqref>AW27:AW33 AY27:AY33 AQ30:AS30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$17:$B$18</xm:f>
           </x14:formula1>
           <xm:sqref>AW38:AW44 AY38:AY44 AQ41:AS41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
           <x14:formula1>
             <xm:f>Matchups!$D$14:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>AN14:AP14 AK5:AK11 AM5:AM11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000E000000}">
           <x14:formula1>
             <xm:f>Matchups!$D$17:$D$18</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Updated Playoff Box Scores, Standings
Data Input to EOD 5/7/24
</commit_message>
<xml_diff>
--- a/2024/Playoffs/Brackets.xlsx
+++ b/2024/Playoffs/Brackets.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\NHLStats\2024\Playoffs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LunchProjects\GitHub\NHLStats\2024\Playoffs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6831DC64-75DB-469C-BC3D-F92807B48C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Matchups" sheetId="3" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="94">
   <si>
     <t>Eastern Conference Playoff Teams</t>
   </si>
@@ -305,12 +304,15 @@
   </si>
   <si>
     <t>Stars Lead 3-2</t>
+  </si>
+  <si>
+    <t>Avalanche Lead 1-0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -680,14 +682,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -695,6 +715,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -709,33 +738,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1016,7 +1018,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1109,18 +1111,18 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41" t="s">
+      <c r="B11" s="43"/>
+      <c r="C11" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41" t="s">
+      <c r="D11" s="43"/>
+      <c r="E11" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="41"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="4" t="s">
         <v>40</v>
       </c>
@@ -1149,18 +1151,18 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="42" t="s">
+      <c r="B13" s="42"/>
+      <c r="C13" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="42" t="s">
+      <c r="D13" s="42"/>
+      <c r="E13" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="43"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1197,14 +1199,14 @@
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="42" t="s">
+      <c r="B16" s="42"/>
+      <c r="C16" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="43"/>
+      <c r="D16" s="42"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1235,10 +1237,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="43"/>
+      <c r="B19" s="42"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1257,10 +1259,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="43"/>
+      <c r="B22" s="42"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -1342,16 +1344,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1359,11 +1361,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="AE28" workbookViewId="0">
+      <selection activeCell="AL42" sqref="AL42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,124 +1410,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="53"/>
-      <c r="Z1" s="51" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="54"/>
+      <c r="Z1" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="53"/>
-      <c r="AF1" s="51" t="s">
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="54"/>
+      <c r="AF1" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AG1" s="52"/>
-      <c r="AH1" s="52"/>
-      <c r="AI1" s="52"/>
-      <c r="AJ1" s="52"/>
-      <c r="AK1" s="52"/>
-      <c r="AL1" s="52"/>
-      <c r="AM1" s="52"/>
-      <c r="AN1" s="52"/>
-      <c r="AO1" s="52"/>
-      <c r="AP1" s="52"/>
-      <c r="AQ1" s="52"/>
-      <c r="AR1" s="52"/>
-      <c r="AS1" s="52"/>
-      <c r="AT1" s="52"/>
-      <c r="AU1" s="52"/>
-      <c r="AV1" s="52"/>
-      <c r="AW1" s="52"/>
-      <c r="AX1" s="52"/>
-      <c r="AY1" s="52"/>
-      <c r="AZ1" s="52"/>
-      <c r="BA1" s="53"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="53"/>
+      <c r="AL1" s="53"/>
+      <c r="AM1" s="53"/>
+      <c r="AN1" s="53"/>
+      <c r="AO1" s="53"/>
+      <c r="AP1" s="53"/>
+      <c r="AQ1" s="53"/>
+      <c r="AR1" s="53"/>
+      <c r="AS1" s="53"/>
+      <c r="AT1" s="53"/>
+      <c r="AU1" s="53"/>
+      <c r="AV1" s="53"/>
+      <c r="AW1" s="53"/>
+      <c r="AX1" s="53"/>
+      <c r="AY1" s="53"/>
+      <c r="AZ1" s="53"/>
+      <c r="BA1" s="54"/>
     </row>
     <row r="2" spans="1:54" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="49"/>
-      <c r="M2" s="47" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="M2" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="49"/>
-      <c r="AI2" s="47" t="s">
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="58"/>
+      <c r="AI2" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="48"/>
-      <c r="AM2" s="48"/>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="49"/>
-      <c r="AU2" s="47" t="s">
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="58"/>
+      <c r="AU2" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="AV2" s="48"/>
-      <c r="AW2" s="48"/>
-      <c r="AX2" s="48"/>
-      <c r="AY2" s="48"/>
-      <c r="AZ2" s="48"/>
-      <c r="BA2" s="49"/>
+      <c r="AV2" s="57"/>
+      <c r="AW2" s="57"/>
+      <c r="AX2" s="57"/>
+      <c r="AY2" s="57"/>
+      <c r="AZ2" s="57"/>
+      <c r="BA2" s="58"/>
     </row>
     <row r="3" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="AI3" s="44" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="AI3" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="AJ3" s="44"/>
-      <c r="AK3" s="44"/>
-      <c r="AL3" s="44"/>
-      <c r="AM3" s="44"/>
-      <c r="AN3" s="44"/>
-      <c r="AO3" s="44"/>
-      <c r="AU3" s="44" t="s">
+      <c r="AJ3" s="50"/>
+      <c r="AK3" s="50"/>
+      <c r="AL3" s="50"/>
+      <c r="AM3" s="50"/>
+      <c r="AN3" s="50"/>
+      <c r="AO3" s="50"/>
+      <c r="AU3" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="AV3" s="44"/>
-      <c r="AW3" s="44"/>
-      <c r="AX3" s="44"/>
-      <c r="AY3" s="44"/>
-      <c r="AZ3" s="44"/>
-      <c r="BA3" s="44"/>
+      <c r="AV3" s="50"/>
+      <c r="AW3" s="50"/>
+      <c r="AX3" s="50"/>
+      <c r="AY3" s="50"/>
+      <c r="AZ3" s="50"/>
+      <c r="BA3" s="50"/>
     </row>
     <row r="4" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -1549,15 +1551,15 @@
       <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="54" t="s">
+      <c r="M4" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="55"/>
-      <c r="S4" s="56"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="46"/>
       <c r="AI4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1866,11 +1868,11 @@
       <c r="G8" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="I8" s="45" t="s">
+      <c r="I8" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
       <c r="M8" s="8">
         <v>3</v>
       </c>
@@ -1901,11 +1903,11 @@
       </c>
       <c r="AN8" s="33"/>
       <c r="AO8" s="34"/>
-      <c r="AQ8" s="45" t="s">
+      <c r="AQ8" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="AR8" s="45"/>
-      <c r="AS8" s="45"/>
+      <c r="AR8" s="51"/>
+      <c r="AS8" s="51"/>
       <c r="AU8" s="40">
         <v>4</v>
       </c>
@@ -2120,15 +2122,15 @@
       <c r="BA11" s="6"/>
     </row>
     <row r="12" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
       <c r="L12" s="12"/>
       <c r="M12" s="8" t="s">
         <v>28</v>
@@ -2143,65 +2145,65 @@
       </c>
       <c r="R12" s="13"/>
       <c r="S12" s="16"/>
-      <c r="AI12" s="44" t="s">
+      <c r="AI12" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AJ12" s="44"/>
-      <c r="AK12" s="44"/>
-      <c r="AL12" s="44"/>
-      <c r="AM12" s="44"/>
-      <c r="AN12" s="44"/>
-      <c r="AO12" s="44"/>
+      <c r="AJ12" s="50"/>
+      <c r="AK12" s="50"/>
+      <c r="AL12" s="50"/>
+      <c r="AM12" s="50"/>
+      <c r="AN12" s="50"/>
+      <c r="AO12" s="50"/>
       <c r="AQ12" s="12"/>
-      <c r="AU12" s="44" t="s">
+      <c r="AU12" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AV12" s="44"/>
-      <c r="AW12" s="44"/>
-      <c r="AX12" s="44"/>
-      <c r="AY12" s="44"/>
-      <c r="AZ12" s="44"/>
-      <c r="BA12" s="44"/>
+      <c r="AV12" s="50"/>
+      <c r="AW12" s="50"/>
+      <c r="AX12" s="50"/>
+      <c r="AY12" s="50"/>
+      <c r="AZ12" s="50"/>
+      <c r="BA12" s="50"/>
     </row>
     <row r="13" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L13" s="12"/>
-      <c r="M13" s="54" t="s">
+      <c r="M13" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="55"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="56"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="46"/>
       <c r="AQ13" s="12"/>
     </row>
     <row r="14" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="AN14" s="45"/>
-      <c r="AO14" s="45"/>
-      <c r="AP14" s="45"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="AN14" s="51"/>
+      <c r="AO14" s="51"/>
+      <c r="AP14" s="51"/>
       <c r="AQ14" s="12"/>
-      <c r="AU14" s="44" t="s">
+      <c r="AU14" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="AV14" s="44"/>
-      <c r="AW14" s="44"/>
-      <c r="AX14" s="44"/>
-      <c r="AY14" s="44"/>
-      <c r="AZ14" s="44"/>
-      <c r="BA14" s="44"/>
+      <c r="AV14" s="50"/>
+      <c r="AW14" s="50"/>
+      <c r="AX14" s="50"/>
+      <c r="AY14" s="50"/>
+      <c r="AZ14" s="50"/>
+      <c r="BA14" s="50"/>
     </row>
     <row r="15" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -2423,19 +2425,19 @@
       <c r="H19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
+      <c r="I19" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
       <c r="L19" s="12"/>
       <c r="O19" s="12"/>
       <c r="AN19" s="12"/>
-      <c r="AQ19" s="46" t="s">
+      <c r="AQ19" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="AR19" s="45"/>
-      <c r="AS19" s="45"/>
+      <c r="AR19" s="51"/>
+      <c r="AS19" s="51"/>
       <c r="AU19" s="40">
         <v>4</v>
       </c>
@@ -2565,52 +2567,52 @@
       <c r="BA22" s="6"/>
     </row>
     <row r="23" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
       <c r="O23" s="12"/>
       <c r="AN23" s="12"/>
-      <c r="AU23" s="44" t="s">
+      <c r="AU23" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AV23" s="44"/>
-      <c r="AW23" s="44"/>
-      <c r="AX23" s="44"/>
-      <c r="AY23" s="44"/>
-      <c r="AZ23" s="44"/>
-      <c r="BA23" s="44"/>
+      <c r="AV23" s="50"/>
+      <c r="AW23" s="50"/>
+      <c r="AX23" s="50"/>
+      <c r="AY23" s="50"/>
+      <c r="AZ23" s="50"/>
+      <c r="BA23" s="50"/>
     </row>
     <row r="24" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O24" s="12"/>
       <c r="AN24" s="12"/>
     </row>
     <row r="25" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
       <c r="O25" s="12"/>
       <c r="AN25" s="12"/>
-      <c r="AU25" s="44" t="s">
+      <c r="AU25" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="AV25" s="44"/>
-      <c r="AW25" s="44"/>
-      <c r="AX25" s="44"/>
-      <c r="AY25" s="44"/>
-      <c r="AZ25" s="44"/>
-      <c r="BA25" s="44"/>
+      <c r="AV25" s="50"/>
+      <c r="AW25" s="50"/>
+      <c r="AX25" s="50"/>
+      <c r="AY25" s="50"/>
+      <c r="AZ25" s="50"/>
+      <c r="BA25" s="50"/>
     </row>
     <row r="26" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="20" t="s">
@@ -2634,24 +2636,24 @@
       <c r="G26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="O26" s="46"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="45"/>
-      <c r="U26" s="45"/>
-      <c r="V26" s="45"/>
-      <c r="W26" s="45"/>
-      <c r="AE26" s="45"/>
-      <c r="AF26" s="45"/>
-      <c r="AG26" s="45"/>
-      <c r="AH26" s="45"/>
-      <c r="AI26" s="45"/>
-      <c r="AJ26" s="45"/>
-      <c r="AK26" s="45"/>
-      <c r="AL26" s="45"/>
-      <c r="AM26" s="50"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="51"/>
+      <c r="S26" s="51"/>
+      <c r="T26" s="51"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="51"/>
+      <c r="AE26" s="51"/>
+      <c r="AF26" s="51"/>
+      <c r="AG26" s="51"/>
+      <c r="AH26" s="51"/>
+      <c r="AI26" s="51"/>
+      <c r="AJ26" s="51"/>
+      <c r="AK26" s="51"/>
+      <c r="AL26" s="51"/>
+      <c r="AM26" s="59"/>
       <c r="AU26" s="20" t="s">
         <v>18</v>
       </c>
@@ -2745,26 +2747,26 @@
         <v>56</v>
       </c>
       <c r="O28" s="12"/>
-      <c r="P28" s="54" t="s">
+      <c r="P28" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="Q28" s="55"/>
-      <c r="R28" s="55"/>
-      <c r="S28" s="55"/>
-      <c r="T28" s="55"/>
-      <c r="U28" s="55"/>
-      <c r="V28" s="56"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="45"/>
+      <c r="S28" s="45"/>
+      <c r="T28" s="45"/>
+      <c r="U28" s="45"/>
+      <c r="V28" s="46"/>
       <c r="X28" s="12"/>
       <c r="AD28" s="13"/>
-      <c r="AF28" s="44" t="s">
+      <c r="AF28" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="AG28" s="44"/>
-      <c r="AH28" s="44"/>
-      <c r="AI28" s="44"/>
-      <c r="AJ28" s="44"/>
-      <c r="AK28" s="44"/>
-      <c r="AL28" s="44"/>
+      <c r="AG28" s="50"/>
+      <c r="AH28" s="50"/>
+      <c r="AI28" s="50"/>
+      <c r="AJ28" s="50"/>
+      <c r="AK28" s="50"/>
+      <c r="AL28" s="50"/>
       <c r="AN28" s="12"/>
       <c r="AU28" s="8">
         <v>2</v>
@@ -2900,11 +2902,11 @@
       <c r="G30" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="I30" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
+      <c r="I30" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="J30" s="51"/>
+      <c r="K30" s="51"/>
       <c r="O30" s="12"/>
       <c r="P30" s="7">
         <v>1</v>
@@ -2927,11 +2929,11 @@
       <c r="AK30" s="25"/>
       <c r="AL30" s="26"/>
       <c r="AN30" s="12"/>
-      <c r="AQ30" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="AR30" s="45"/>
-      <c r="AS30" s="45"/>
+      <c r="AQ30" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR30" s="51"/>
+      <c r="AS30" s="51"/>
       <c r="AU30" s="40">
         <v>4</v>
       </c>
@@ -3151,15 +3153,15 @@
       <c r="BA33" s="6"/>
     </row>
     <row r="34" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
       <c r="L34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="8" t="s">
@@ -3184,15 +3186,15 @@
       <c r="AL34" s="16"/>
       <c r="AN34" s="12"/>
       <c r="AQ34" s="12"/>
-      <c r="AU34" s="44" t="s">
+      <c r="AU34" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AV34" s="44"/>
-      <c r="AW34" s="44"/>
-      <c r="AX34" s="44"/>
-      <c r="AY34" s="44"/>
-      <c r="AZ34" s="44"/>
-      <c r="BA34" s="44"/>
+      <c r="AV34" s="50"/>
+      <c r="AW34" s="50"/>
+      <c r="AX34" s="50"/>
+      <c r="AY34" s="50"/>
+      <c r="AZ34" s="50"/>
+      <c r="BA34" s="50"/>
     </row>
     <row r="35" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L35" s="12"/>
@@ -3221,18 +3223,18 @@
       <c r="AQ35" s="12"/>
     </row>
     <row r="36" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="51"/>
       <c r="O36" s="12"/>
       <c r="P36" s="8" t="s">
         <v>28</v>
@@ -3254,19 +3256,19 @@
       <c r="AJ36" s="37"/>
       <c r="AK36" s="38"/>
       <c r="AL36" s="39"/>
-      <c r="AN36" s="46"/>
-      <c r="AO36" s="45"/>
-      <c r="AP36" s="45"/>
+      <c r="AN36" s="55"/>
+      <c r="AO36" s="51"/>
+      <c r="AP36" s="51"/>
       <c r="AQ36" s="12"/>
-      <c r="AU36" s="44" t="s">
+      <c r="AU36" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="AV36" s="44"/>
-      <c r="AW36" s="44"/>
-      <c r="AX36" s="44"/>
-      <c r="AY36" s="44"/>
-      <c r="AZ36" s="44"/>
-      <c r="BA36" s="44"/>
+      <c r="AV36" s="50"/>
+      <c r="AW36" s="50"/>
+      <c r="AX36" s="50"/>
+      <c r="AY36" s="50"/>
+      <c r="AZ36" s="50"/>
+      <c r="BA36" s="50"/>
     </row>
     <row r="37" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="20" t="s">
@@ -3291,31 +3293,31 @@
         <v>25</v>
       </c>
       <c r="L37" s="12"/>
-      <c r="P37" s="57" t="s">
+      <c r="P37" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Q37" s="58"/>
-      <c r="R37" s="58"/>
-      <c r="S37" s="58"/>
-      <c r="T37" s="58"/>
-      <c r="U37" s="58"/>
-      <c r="V37" s="59"/>
-      <c r="X37" s="46"/>
-      <c r="Y37" s="45"/>
-      <c r="Z37" s="45"/>
-      <c r="AA37" s="45"/>
-      <c r="AB37" s="45"/>
-      <c r="AC37" s="45"/>
-      <c r="AD37" s="50"/>
-      <c r="AF37" s="44" t="s">
+      <c r="Q37" s="48"/>
+      <c r="R37" s="48"/>
+      <c r="S37" s="48"/>
+      <c r="T37" s="48"/>
+      <c r="U37" s="48"/>
+      <c r="V37" s="49"/>
+      <c r="X37" s="55"/>
+      <c r="Y37" s="51"/>
+      <c r="Z37" s="51"/>
+      <c r="AA37" s="51"/>
+      <c r="AB37" s="51"/>
+      <c r="AC37" s="51"/>
+      <c r="AD37" s="59"/>
+      <c r="AF37" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AG37" s="44"/>
-      <c r="AH37" s="44"/>
-      <c r="AI37" s="44"/>
-      <c r="AJ37" s="44"/>
-      <c r="AK37" s="44"/>
-      <c r="AL37" s="44"/>
+      <c r="AG37" s="50"/>
+      <c r="AH37" s="50"/>
+      <c r="AI37" s="50"/>
+      <c r="AJ37" s="50"/>
+      <c r="AK37" s="50"/>
+      <c r="AL37" s="50"/>
       <c r="AQ37" s="12"/>
       <c r="AU37" s="3" t="s">
         <v>18</v>
@@ -3411,33 +3413,33 @@
         <v>59</v>
       </c>
       <c r="L39" s="12"/>
-      <c r="M39" s="54" t="s">
+      <c r="M39" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="N39" s="55"/>
-      <c r="O39" s="55"/>
-      <c r="P39" s="55"/>
-      <c r="Q39" s="55"/>
-      <c r="R39" s="55"/>
-      <c r="S39" s="56"/>
-      <c r="X39" s="44" t="s">
+      <c r="N39" s="45"/>
+      <c r="O39" s="45"/>
+      <c r="P39" s="45"/>
+      <c r="Q39" s="45"/>
+      <c r="R39" s="45"/>
+      <c r="S39" s="46"/>
+      <c r="X39" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="Y39" s="44"/>
-      <c r="Z39" s="44"/>
-      <c r="AA39" s="44"/>
-      <c r="AB39" s="44"/>
-      <c r="AC39" s="44"/>
-      <c r="AD39" s="44"/>
-      <c r="AI39" s="44" t="s">
+      <c r="Y39" s="50"/>
+      <c r="Z39" s="50"/>
+      <c r="AA39" s="50"/>
+      <c r="AB39" s="50"/>
+      <c r="AC39" s="50"/>
+      <c r="AD39" s="50"/>
+      <c r="AI39" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="AJ39" s="44"/>
-      <c r="AK39" s="44"/>
-      <c r="AL39" s="44"/>
-      <c r="AM39" s="44"/>
-      <c r="AN39" s="44"/>
-      <c r="AO39" s="44"/>
+      <c r="AJ39" s="50"/>
+      <c r="AK39" s="50"/>
+      <c r="AL39" s="50"/>
+      <c r="AM39" s="50"/>
+      <c r="AN39" s="50"/>
+      <c r="AO39" s="50"/>
       <c r="AQ39" s="12"/>
       <c r="AU39" s="8">
         <v>2</v>
@@ -3595,11 +3597,11 @@
       <c r="G41" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I41" s="45" t="s">
+      <c r="I41" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="J41" s="45"/>
-      <c r="K41" s="45"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="51"/>
       <c r="L41" s="12"/>
       <c r="M41" s="7">
         <v>1</v>
@@ -3640,17 +3642,26 @@
       <c r="AK41" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="AL41" s="25"/>
+      <c r="AL41" s="25">
+        <v>4</v>
+      </c>
       <c r="AM41" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AN41" s="25"/>
-      <c r="AO41" s="26"/>
-      <c r="AQ41" s="46" t="s">
+      <c r="AN41" s="25">
+        <v>3</v>
+      </c>
+      <c r="AO41" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP41" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ41" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="AR41" s="45"/>
-      <c r="AS41" s="45"/>
+      <c r="AR41" s="51"/>
+      <c r="AS41" s="51"/>
       <c r="AU41" s="8">
         <v>4</v>
       </c>
@@ -3907,15 +3918,15 @@
       </c>
     </row>
     <row r="45" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="44" t="s">
+      <c r="A45" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
       <c r="M45" s="8" t="s">
         <v>27</v>
       </c>
@@ -3951,15 +3962,15 @@
       </c>
       <c r="AN45" s="13"/>
       <c r="AO45" s="16"/>
-      <c r="AU45" s="44" t="s">
+      <c r="AU45" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AV45" s="44"/>
-      <c r="AW45" s="44"/>
-      <c r="AX45" s="44"/>
-      <c r="AY45" s="44"/>
-      <c r="AZ45" s="44"/>
-      <c r="BA45" s="44"/>
+      <c r="AV45" s="50"/>
+      <c r="AW45" s="50"/>
+      <c r="AX45" s="50"/>
+      <c r="AY45" s="50"/>
+      <c r="AZ45" s="50"/>
+      <c r="BA45" s="50"/>
     </row>
     <row r="46" spans="1:54" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="M46" s="8" t="s">
@@ -4036,45 +4047,65 @@
       <c r="AO47" s="6"/>
     </row>
     <row r="48" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M48" s="54" t="s">
+      <c r="M48" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="N48" s="55"/>
-      <c r="O48" s="55"/>
-      <c r="P48" s="55"/>
-      <c r="Q48" s="55"/>
-      <c r="R48" s="55"/>
-      <c r="S48" s="56"/>
-      <c r="X48" s="44" t="s">
+      <c r="N48" s="45"/>
+      <c r="O48" s="45"/>
+      <c r="P48" s="45"/>
+      <c r="Q48" s="45"/>
+      <c r="R48" s="45"/>
+      <c r="S48" s="46"/>
+      <c r="X48" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="Y48" s="44"/>
-      <c r="Z48" s="44"/>
-      <c r="AA48" s="44"/>
-      <c r="AB48" s="44"/>
-      <c r="AC48" s="44"/>
-      <c r="AD48" s="44"/>
-      <c r="AI48" s="44" t="s">
+      <c r="Y48" s="50"/>
+      <c r="Z48" s="50"/>
+      <c r="AA48" s="50"/>
+      <c r="AB48" s="50"/>
+      <c r="AC48" s="50"/>
+      <c r="AD48" s="50"/>
+      <c r="AI48" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AJ48" s="44"/>
-      <c r="AK48" s="44"/>
-      <c r="AL48" s="44"/>
-      <c r="AM48" s="44"/>
-      <c r="AN48" s="44"/>
-      <c r="AO48" s="44"/>
+      <c r="AJ48" s="50"/>
+      <c r="AK48" s="50"/>
+      <c r="AL48" s="50"/>
+      <c r="AM48" s="50"/>
+      <c r="AN48" s="50"/>
+      <c r="AO48" s="50"/>
     </row>
     <row r="49" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="M48:S48"/>
-    <mergeCell ref="M39:S39"/>
-    <mergeCell ref="P37:V37"/>
-    <mergeCell ref="P28:V28"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="AU45:BA45"/>
+    <mergeCell ref="AF28:AL28"/>
+    <mergeCell ref="AF37:AL37"/>
+    <mergeCell ref="AQ30:AS30"/>
+    <mergeCell ref="AQ41:AS41"/>
+    <mergeCell ref="AU34:BA34"/>
+    <mergeCell ref="AU36:BA36"/>
+    <mergeCell ref="AU2:BA2"/>
+    <mergeCell ref="AU3:BA3"/>
+    <mergeCell ref="AU12:BA12"/>
+    <mergeCell ref="AU14:BA14"/>
+    <mergeCell ref="AU23:BA23"/>
+    <mergeCell ref="X37:AD37"/>
+    <mergeCell ref="AE26:AM26"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="X39:AD39"/>
+    <mergeCell ref="X48:AD48"/>
+    <mergeCell ref="AF1:BA1"/>
+    <mergeCell ref="AI2:AO2"/>
+    <mergeCell ref="AI3:AO3"/>
+    <mergeCell ref="AI12:AO12"/>
+    <mergeCell ref="AI39:AO39"/>
+    <mergeCell ref="AU25:BA25"/>
+    <mergeCell ref="AI48:AO48"/>
+    <mergeCell ref="AN14:AP14"/>
+    <mergeCell ref="AN36:AP36"/>
+    <mergeCell ref="AQ8:AS8"/>
+    <mergeCell ref="AQ19:AS19"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="O26:W26"/>
     <mergeCell ref="I41:K41"/>
@@ -4091,125 +4122,105 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I19:K19"/>
     <mergeCell ref="A25:G25"/>
-    <mergeCell ref="X37:AD37"/>
-    <mergeCell ref="AE26:AM26"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="X39:AD39"/>
-    <mergeCell ref="X48:AD48"/>
-    <mergeCell ref="AF1:BA1"/>
-    <mergeCell ref="AI2:AO2"/>
-    <mergeCell ref="AI3:AO3"/>
-    <mergeCell ref="AI12:AO12"/>
-    <mergeCell ref="AI39:AO39"/>
-    <mergeCell ref="AU25:BA25"/>
-    <mergeCell ref="AI48:AO48"/>
-    <mergeCell ref="AN14:AP14"/>
-    <mergeCell ref="AN36:AP36"/>
-    <mergeCell ref="AQ8:AS8"/>
-    <mergeCell ref="AQ19:AS19"/>
-    <mergeCell ref="AU2:BA2"/>
-    <mergeCell ref="AU3:BA3"/>
-    <mergeCell ref="AU12:BA12"/>
-    <mergeCell ref="AU14:BA14"/>
-    <mergeCell ref="AU23:BA23"/>
-    <mergeCell ref="AU45:BA45"/>
-    <mergeCell ref="AF28:AL28"/>
-    <mergeCell ref="AF37:AL37"/>
-    <mergeCell ref="AQ30:AS30"/>
-    <mergeCell ref="AQ41:AS41"/>
-    <mergeCell ref="AU34:BA34"/>
-    <mergeCell ref="AU36:BA36"/>
+    <mergeCell ref="M48:S48"/>
+    <mergeCell ref="M39:S39"/>
+    <mergeCell ref="P37:V37"/>
+    <mergeCell ref="P28:V28"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="A34:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="15">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$A$14:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C11 E5:E11 I8:K8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$A$20:$A$21</xm:f>
           </x14:formula1>
           <xm:sqref>C16:C22 E16:E22 I19:K19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$A$23:$A$24</xm:f>
           </x14:formula1>
           <xm:sqref>C27:C33 E27:E33 I30:K30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$A$17:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>C38:C44 E38:E44 I41:K41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$C$14:$C$15</xm:f>
           </x14:formula1>
           <xm:sqref>L14:N14 Q6:Q12 O6:O12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$C$17:$C$18</xm:f>
           </x14:formula1>
           <xm:sqref>L36:N36 Q41:Q47 O41:O47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$E$14:$E$15</xm:f>
           </x14:formula1>
           <xm:sqref>T30:T36 Q30:R36 O26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$F$14:$F$15</xm:f>
           </x14:formula1>
           <xm:sqref>AE26:AM26 AJ30:AJ36 AH30:AH36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$G$13:$G$14</xm:f>
           </x14:formula1>
           <xm:sqref>X37:AD37 Z41:Z47 AB41:AB47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$B$14:$B$15</xm:f>
           </x14:formula1>
           <xm:sqref>AW5:AW11 AY5:AY11 AQ8:AS8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$B$20:$B$21</xm:f>
           </x14:formula1>
           <xm:sqref>AW16:AW22 AY16:AY22 AQ19:AS19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$B$23:$B$24</xm:f>
           </x14:formula1>
           <xm:sqref>AW27:AW33 AY27:AY33 AQ30:AS30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$B$17:$B$18</xm:f>
           </x14:formula1>
           <xm:sqref>AW38:AW44 AY38:AY44 AQ41:AS41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$D$14:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>AN14:AP14 AK5:AK11 AM5:AM11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000E000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$D$17:$D$18</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Updated Box Scores, Bracket
Data Input to first game EOD 5/16/24
</commit_message>
<xml_diff>
--- a/2024/Playoffs/Brackets.xlsx
+++ b/2024/Playoffs/Brackets.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LunchProjects\GitHub\NHLStats\2024\Playoffs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\NHLStats\2024\Playoffs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E915EF8-49BC-436E-A73D-F2FE2236F91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matchups" sheetId="3" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="101">
   <si>
     <t>Eastern Conference Playoff Teams</t>
   </si>
@@ -325,12 +326,15 @@
   </si>
   <si>
     <t>Panthers Lead 3-2</t>
+  </si>
+  <si>
+    <t>Rangers Win 4-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -700,14 +704,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -715,6 +737,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -729,33 +760,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1036,11 +1040,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,18 +1133,18 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41" t="s">
+      <c r="B11" s="43"/>
+      <c r="C11" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41" t="s">
+      <c r="D11" s="43"/>
+      <c r="E11" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="41"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="4" t="s">
         <v>40</v>
       </c>
@@ -1169,18 +1173,18 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="42" t="s">
+      <c r="B13" s="42"/>
+      <c r="C13" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="42" t="s">
+      <c r="D13" s="42"/>
+      <c r="E13" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="43"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1196,7 +1200,9 @@
       <c r="D14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
     </row>
@@ -1217,14 +1223,14 @@
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="42" t="s">
+      <c r="B16" s="42"/>
+      <c r="C16" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="43"/>
+      <c r="D16" s="42"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1255,10 +1261,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="43"/>
+      <c r="B19" s="42"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1277,10 +1283,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="43"/>
+      <c r="B22" s="42"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -1362,16 +1368,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1379,11 +1385,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BB49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AL9" sqref="AL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,124 +1434,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="53"/>
-      <c r="Z1" s="51" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="54"/>
+      <c r="Z1" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="53"/>
-      <c r="AF1" s="51" t="s">
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="54"/>
+      <c r="AF1" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AG1" s="52"/>
-      <c r="AH1" s="52"/>
-      <c r="AI1" s="52"/>
-      <c r="AJ1" s="52"/>
-      <c r="AK1" s="52"/>
-      <c r="AL1" s="52"/>
-      <c r="AM1" s="52"/>
-      <c r="AN1" s="52"/>
-      <c r="AO1" s="52"/>
-      <c r="AP1" s="52"/>
-      <c r="AQ1" s="52"/>
-      <c r="AR1" s="52"/>
-      <c r="AS1" s="52"/>
-      <c r="AT1" s="52"/>
-      <c r="AU1" s="52"/>
-      <c r="AV1" s="52"/>
-      <c r="AW1" s="52"/>
-      <c r="AX1" s="52"/>
-      <c r="AY1" s="52"/>
-      <c r="AZ1" s="52"/>
-      <c r="BA1" s="53"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="53"/>
+      <c r="AL1" s="53"/>
+      <c r="AM1" s="53"/>
+      <c r="AN1" s="53"/>
+      <c r="AO1" s="53"/>
+      <c r="AP1" s="53"/>
+      <c r="AQ1" s="53"/>
+      <c r="AR1" s="53"/>
+      <c r="AS1" s="53"/>
+      <c r="AT1" s="53"/>
+      <c r="AU1" s="53"/>
+      <c r="AV1" s="53"/>
+      <c r="AW1" s="53"/>
+      <c r="AX1" s="53"/>
+      <c r="AY1" s="53"/>
+      <c r="AZ1" s="53"/>
+      <c r="BA1" s="54"/>
     </row>
     <row r="2" spans="1:54" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="49"/>
-      <c r="M2" s="47" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="M2" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="49"/>
-      <c r="AI2" s="47" t="s">
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="58"/>
+      <c r="AI2" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="48"/>
-      <c r="AM2" s="48"/>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="49"/>
-      <c r="AU2" s="47" t="s">
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="58"/>
+      <c r="AU2" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="AV2" s="48"/>
-      <c r="AW2" s="48"/>
-      <c r="AX2" s="48"/>
-      <c r="AY2" s="48"/>
-      <c r="AZ2" s="48"/>
-      <c r="BA2" s="49"/>
+      <c r="AV2" s="57"/>
+      <c r="AW2" s="57"/>
+      <c r="AX2" s="57"/>
+      <c r="AY2" s="57"/>
+      <c r="AZ2" s="57"/>
+      <c r="BA2" s="58"/>
     </row>
     <row r="3" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="AI3" s="44" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="AI3" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="AJ3" s="44"/>
-      <c r="AK3" s="44"/>
-      <c r="AL3" s="44"/>
-      <c r="AM3" s="44"/>
-      <c r="AN3" s="44"/>
-      <c r="AO3" s="44"/>
-      <c r="AU3" s="44" t="s">
+      <c r="AJ3" s="50"/>
+      <c r="AK3" s="50"/>
+      <c r="AL3" s="50"/>
+      <c r="AM3" s="50"/>
+      <c r="AN3" s="50"/>
+      <c r="AO3" s="50"/>
+      <c r="AU3" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="AV3" s="44"/>
-      <c r="AW3" s="44"/>
-      <c r="AX3" s="44"/>
-      <c r="AY3" s="44"/>
-      <c r="AZ3" s="44"/>
-      <c r="BA3" s="44"/>
+      <c r="AV3" s="50"/>
+      <c r="AW3" s="50"/>
+      <c r="AX3" s="50"/>
+      <c r="AY3" s="50"/>
+      <c r="AZ3" s="50"/>
+      <c r="BA3" s="50"/>
     </row>
     <row r="4" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -1569,15 +1575,15 @@
       <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="54" t="s">
+      <c r="M4" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="55"/>
-      <c r="S4" s="56"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="46"/>
       <c r="AI4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1907,11 +1913,11 @@
       <c r="G8" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="I8" s="45" t="s">
+      <c r="I8" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
       <c r="M8" s="8">
         <v>3</v>
       </c>
@@ -1957,11 +1963,11 @@
       <c r="AO8" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="AQ8" s="45" t="s">
+      <c r="AQ8" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="AR8" s="45"/>
-      <c r="AS8" s="45"/>
+      <c r="AR8" s="51"/>
+      <c r="AS8" s="51"/>
       <c r="AU8" s="40">
         <v>4</v>
       </c>
@@ -2159,12 +2165,18 @@
       <c r="O11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="13"/>
+      <c r="P11" s="13">
+        <v>5</v>
+      </c>
       <c r="Q11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="R11" s="13"/>
-      <c r="S11" s="16"/>
+      <c r="R11" s="13">
+        <v>3</v>
+      </c>
+      <c r="S11" s="16" t="s">
+        <v>100</v>
+      </c>
       <c r="AI11" s="9" t="s">
         <v>28</v>
       </c>
@@ -2194,15 +2206,15 @@
       <c r="BA11" s="6"/>
     </row>
     <row r="12" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
       <c r="L12" s="12"/>
       <c r="M12" s="8" t="s">
         <v>28</v>
@@ -2217,65 +2229,67 @@
       </c>
       <c r="R12" s="13"/>
       <c r="S12" s="16"/>
-      <c r="AI12" s="44" t="s">
+      <c r="AI12" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AJ12" s="44"/>
-      <c r="AK12" s="44"/>
-      <c r="AL12" s="44"/>
-      <c r="AM12" s="44"/>
-      <c r="AN12" s="44"/>
-      <c r="AO12" s="44"/>
+      <c r="AJ12" s="50"/>
+      <c r="AK12" s="50"/>
+      <c r="AL12" s="50"/>
+      <c r="AM12" s="50"/>
+      <c r="AN12" s="50"/>
+      <c r="AO12" s="50"/>
       <c r="AQ12" s="12"/>
-      <c r="AU12" s="44" t="s">
+      <c r="AU12" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AV12" s="44"/>
-      <c r="AW12" s="44"/>
-      <c r="AX12" s="44"/>
-      <c r="AY12" s="44"/>
-      <c r="AZ12" s="44"/>
-      <c r="BA12" s="44"/>
+      <c r="AV12" s="50"/>
+      <c r="AW12" s="50"/>
+      <c r="AX12" s="50"/>
+      <c r="AY12" s="50"/>
+      <c r="AZ12" s="50"/>
+      <c r="BA12" s="50"/>
     </row>
     <row r="13" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L13" s="12"/>
-      <c r="M13" s="54" t="s">
+      <c r="M13" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="55"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="56"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="46"/>
       <c r="AQ13" s="12"/>
     </row>
     <row r="14" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="AN14" s="45"/>
-      <c r="AO14" s="45"/>
-      <c r="AP14" s="45"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="L14" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="AN14" s="51"/>
+      <c r="AO14" s="51"/>
+      <c r="AP14" s="51"/>
       <c r="AQ14" s="12"/>
-      <c r="AU14" s="44" t="s">
+      <c r="AU14" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="AV14" s="44"/>
-      <c r="AW14" s="44"/>
-      <c r="AX14" s="44"/>
-      <c r="AY14" s="44"/>
-      <c r="AZ14" s="44"/>
-      <c r="BA14" s="44"/>
+      <c r="AV14" s="50"/>
+      <c r="AW14" s="50"/>
+      <c r="AX14" s="50"/>
+      <c r="AY14" s="50"/>
+      <c r="AZ14" s="50"/>
+      <c r="BA14" s="50"/>
     </row>
     <row r="15" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -2497,19 +2511,19 @@
       <c r="H19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
+      <c r="I19" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
       <c r="L19" s="12"/>
       <c r="O19" s="12"/>
       <c r="AN19" s="12"/>
-      <c r="AQ19" s="46" t="s">
+      <c r="AQ19" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="AR19" s="45"/>
-      <c r="AS19" s="45"/>
+      <c r="AR19" s="51"/>
+      <c r="AS19" s="51"/>
       <c r="AU19" s="40">
         <v>4</v>
       </c>
@@ -2639,52 +2653,52 @@
       <c r="BA22" s="6"/>
     </row>
     <row r="23" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
       <c r="O23" s="12"/>
       <c r="AN23" s="12"/>
-      <c r="AU23" s="44" t="s">
+      <c r="AU23" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AV23" s="44"/>
-      <c r="AW23" s="44"/>
-      <c r="AX23" s="44"/>
-      <c r="AY23" s="44"/>
-      <c r="AZ23" s="44"/>
-      <c r="BA23" s="44"/>
+      <c r="AV23" s="50"/>
+      <c r="AW23" s="50"/>
+      <c r="AX23" s="50"/>
+      <c r="AY23" s="50"/>
+      <c r="AZ23" s="50"/>
+      <c r="BA23" s="50"/>
     </row>
     <row r="24" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O24" s="12"/>
       <c r="AN24" s="12"/>
     </row>
     <row r="25" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
       <c r="O25" s="12"/>
       <c r="AN25" s="12"/>
-      <c r="AU25" s="44" t="s">
+      <c r="AU25" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="AV25" s="44"/>
-      <c r="AW25" s="44"/>
-      <c r="AX25" s="44"/>
-      <c r="AY25" s="44"/>
-      <c r="AZ25" s="44"/>
-      <c r="BA25" s="44"/>
+      <c r="AV25" s="50"/>
+      <c r="AW25" s="50"/>
+      <c r="AX25" s="50"/>
+      <c r="AY25" s="50"/>
+      <c r="AZ25" s="50"/>
+      <c r="BA25" s="50"/>
     </row>
     <row r="26" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="20" t="s">
@@ -2708,24 +2722,24 @@
       <c r="G26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="O26" s="46"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="45"/>
-      <c r="U26" s="45"/>
-      <c r="V26" s="45"/>
-      <c r="W26" s="45"/>
-      <c r="AE26" s="45"/>
-      <c r="AF26" s="45"/>
-      <c r="AG26" s="45"/>
-      <c r="AH26" s="45"/>
-      <c r="AI26" s="45"/>
-      <c r="AJ26" s="45"/>
-      <c r="AK26" s="45"/>
-      <c r="AL26" s="45"/>
-      <c r="AM26" s="50"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="51"/>
+      <c r="S26" s="51"/>
+      <c r="T26" s="51"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="51"/>
+      <c r="AE26" s="51"/>
+      <c r="AF26" s="51"/>
+      <c r="AG26" s="51"/>
+      <c r="AH26" s="51"/>
+      <c r="AI26" s="51"/>
+      <c r="AJ26" s="51"/>
+      <c r="AK26" s="51"/>
+      <c r="AL26" s="51"/>
+      <c r="AM26" s="59"/>
       <c r="AU26" s="20" t="s">
         <v>18</v>
       </c>
@@ -2819,26 +2833,26 @@
         <v>56</v>
       </c>
       <c r="O28" s="12"/>
-      <c r="P28" s="54" t="s">
+      <c r="P28" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="Q28" s="55"/>
-      <c r="R28" s="55"/>
-      <c r="S28" s="55"/>
-      <c r="T28" s="55"/>
-      <c r="U28" s="55"/>
-      <c r="V28" s="56"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="45"/>
+      <c r="S28" s="45"/>
+      <c r="T28" s="45"/>
+      <c r="U28" s="45"/>
+      <c r="V28" s="46"/>
       <c r="X28" s="12"/>
       <c r="AD28" s="13"/>
-      <c r="AF28" s="44" t="s">
+      <c r="AF28" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="AG28" s="44"/>
-      <c r="AH28" s="44"/>
-      <c r="AI28" s="44"/>
-      <c r="AJ28" s="44"/>
-      <c r="AK28" s="44"/>
-      <c r="AL28" s="44"/>
+      <c r="AG28" s="50"/>
+      <c r="AH28" s="50"/>
+      <c r="AI28" s="50"/>
+      <c r="AJ28" s="50"/>
+      <c r="AK28" s="50"/>
+      <c r="AL28" s="50"/>
       <c r="AN28" s="12"/>
       <c r="AU28" s="8">
         <v>2</v>
@@ -2974,11 +2988,11 @@
       <c r="G30" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="I30" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
+      <c r="I30" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="J30" s="51"/>
+      <c r="K30" s="51"/>
       <c r="O30" s="12"/>
       <c r="P30" s="7">
         <v>1</v>
@@ -3001,11 +3015,11 @@
       <c r="AK30" s="25"/>
       <c r="AL30" s="26"/>
       <c r="AN30" s="12"/>
-      <c r="AQ30" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="AR30" s="45"/>
-      <c r="AS30" s="45"/>
+      <c r="AQ30" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR30" s="51"/>
+      <c r="AS30" s="51"/>
       <c r="AU30" s="40">
         <v>4</v>
       </c>
@@ -3225,15 +3239,15 @@
       <c r="BA33" s="6"/>
     </row>
     <row r="34" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
       <c r="L34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="8" t="s">
@@ -3258,15 +3272,15 @@
       <c r="AL34" s="16"/>
       <c r="AN34" s="12"/>
       <c r="AQ34" s="12"/>
-      <c r="AU34" s="44" t="s">
+      <c r="AU34" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AV34" s="44"/>
-      <c r="AW34" s="44"/>
-      <c r="AX34" s="44"/>
-      <c r="AY34" s="44"/>
-      <c r="AZ34" s="44"/>
-      <c r="BA34" s="44"/>
+      <c r="AV34" s="50"/>
+      <c r="AW34" s="50"/>
+      <c r="AX34" s="50"/>
+      <c r="AY34" s="50"/>
+      <c r="AZ34" s="50"/>
+      <c r="BA34" s="50"/>
     </row>
     <row r="35" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L35" s="12"/>
@@ -3295,18 +3309,18 @@
       <c r="AQ35" s="12"/>
     </row>
     <row r="36" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="51"/>
       <c r="O36" s="12"/>
       <c r="P36" s="8" t="s">
         <v>28</v>
@@ -3328,19 +3342,19 @@
       <c r="AJ36" s="37"/>
       <c r="AK36" s="38"/>
       <c r="AL36" s="39"/>
-      <c r="AN36" s="46"/>
-      <c r="AO36" s="45"/>
-      <c r="AP36" s="45"/>
+      <c r="AN36" s="55"/>
+      <c r="AO36" s="51"/>
+      <c r="AP36" s="51"/>
       <c r="AQ36" s="12"/>
-      <c r="AU36" s="44" t="s">
+      <c r="AU36" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="AV36" s="44"/>
-      <c r="AW36" s="44"/>
-      <c r="AX36" s="44"/>
-      <c r="AY36" s="44"/>
-      <c r="AZ36" s="44"/>
-      <c r="BA36" s="44"/>
+      <c r="AV36" s="50"/>
+      <c r="AW36" s="50"/>
+      <c r="AX36" s="50"/>
+      <c r="AY36" s="50"/>
+      <c r="AZ36" s="50"/>
+      <c r="BA36" s="50"/>
     </row>
     <row r="37" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="20" t="s">
@@ -3365,31 +3379,31 @@
         <v>25</v>
       </c>
       <c r="L37" s="12"/>
-      <c r="P37" s="57" t="s">
+      <c r="P37" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Q37" s="58"/>
-      <c r="R37" s="58"/>
-      <c r="S37" s="58"/>
-      <c r="T37" s="58"/>
-      <c r="U37" s="58"/>
-      <c r="V37" s="59"/>
-      <c r="X37" s="46"/>
-      <c r="Y37" s="45"/>
-      <c r="Z37" s="45"/>
-      <c r="AA37" s="45"/>
-      <c r="AB37" s="45"/>
-      <c r="AC37" s="45"/>
-      <c r="AD37" s="50"/>
-      <c r="AF37" s="44" t="s">
+      <c r="Q37" s="48"/>
+      <c r="R37" s="48"/>
+      <c r="S37" s="48"/>
+      <c r="T37" s="48"/>
+      <c r="U37" s="48"/>
+      <c r="V37" s="49"/>
+      <c r="X37" s="55"/>
+      <c r="Y37" s="51"/>
+      <c r="Z37" s="51"/>
+      <c r="AA37" s="51"/>
+      <c r="AB37" s="51"/>
+      <c r="AC37" s="51"/>
+      <c r="AD37" s="59"/>
+      <c r="AF37" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AG37" s="44"/>
-      <c r="AH37" s="44"/>
-      <c r="AI37" s="44"/>
-      <c r="AJ37" s="44"/>
-      <c r="AK37" s="44"/>
-      <c r="AL37" s="44"/>
+      <c r="AG37" s="50"/>
+      <c r="AH37" s="50"/>
+      <c r="AI37" s="50"/>
+      <c r="AJ37" s="50"/>
+      <c r="AK37" s="50"/>
+      <c r="AL37" s="50"/>
       <c r="AQ37" s="12"/>
       <c r="AU37" s="3" t="s">
         <v>18</v>
@@ -3485,33 +3499,33 @@
         <v>59</v>
       </c>
       <c r="L39" s="12"/>
-      <c r="M39" s="54" t="s">
+      <c r="M39" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="N39" s="55"/>
-      <c r="O39" s="55"/>
-      <c r="P39" s="55"/>
-      <c r="Q39" s="55"/>
-      <c r="R39" s="55"/>
-      <c r="S39" s="56"/>
-      <c r="X39" s="44" t="s">
+      <c r="N39" s="45"/>
+      <c r="O39" s="45"/>
+      <c r="P39" s="45"/>
+      <c r="Q39" s="45"/>
+      <c r="R39" s="45"/>
+      <c r="S39" s="46"/>
+      <c r="X39" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="Y39" s="44"/>
-      <c r="Z39" s="44"/>
-      <c r="AA39" s="44"/>
-      <c r="AB39" s="44"/>
-      <c r="AC39" s="44"/>
-      <c r="AD39" s="44"/>
-      <c r="AI39" s="44" t="s">
+      <c r="Y39" s="50"/>
+      <c r="Z39" s="50"/>
+      <c r="AA39" s="50"/>
+      <c r="AB39" s="50"/>
+      <c r="AC39" s="50"/>
+      <c r="AD39" s="50"/>
+      <c r="AI39" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="AJ39" s="44"/>
-      <c r="AK39" s="44"/>
-      <c r="AL39" s="44"/>
-      <c r="AM39" s="44"/>
-      <c r="AN39" s="44"/>
-      <c r="AO39" s="44"/>
+      <c r="AJ39" s="50"/>
+      <c r="AK39" s="50"/>
+      <c r="AL39" s="50"/>
+      <c r="AM39" s="50"/>
+      <c r="AN39" s="50"/>
+      <c r="AO39" s="50"/>
       <c r="AQ39" s="12"/>
       <c r="AU39" s="8">
         <v>2</v>
@@ -3669,11 +3683,11 @@
       <c r="G41" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I41" s="45" t="s">
+      <c r="I41" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="J41" s="45"/>
-      <c r="K41" s="45"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="51"/>
       <c r="L41" s="12"/>
       <c r="M41" s="7">
         <v>1</v>
@@ -3729,11 +3743,11 @@
       <c r="AP41" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AQ41" s="46" t="s">
+      <c r="AQ41" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="AR41" s="45"/>
-      <c r="AS41" s="45"/>
+      <c r="AR41" s="51"/>
+      <c r="AS41" s="51"/>
       <c r="AU41" s="8">
         <v>4</v>
       </c>
@@ -4026,15 +4040,15 @@
       </c>
     </row>
     <row r="45" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="44" t="s">
+      <c r="A45" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
       <c r="M45" s="8" t="s">
         <v>27</v>
       </c>
@@ -4086,15 +4100,15 @@
       <c r="AO45" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="AU45" s="44" t="s">
+      <c r="AU45" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AV45" s="44"/>
-      <c r="AW45" s="44"/>
-      <c r="AX45" s="44"/>
-      <c r="AY45" s="44"/>
-      <c r="AZ45" s="44"/>
-      <c r="BA45" s="44"/>
+      <c r="AV45" s="50"/>
+      <c r="AW45" s="50"/>
+      <c r="AX45" s="50"/>
+      <c r="AY45" s="50"/>
+      <c r="AZ45" s="50"/>
+      <c r="BA45" s="50"/>
     </row>
     <row r="46" spans="1:54" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="M46" s="8" t="s">
@@ -4175,45 +4189,65 @@
       <c r="AO47" s="6"/>
     </row>
     <row r="48" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M48" s="54" t="s">
+      <c r="M48" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="N48" s="55"/>
-      <c r="O48" s="55"/>
-      <c r="P48" s="55"/>
-      <c r="Q48" s="55"/>
-      <c r="R48" s="55"/>
-      <c r="S48" s="56"/>
-      <c r="X48" s="44" t="s">
+      <c r="N48" s="45"/>
+      <c r="O48" s="45"/>
+      <c r="P48" s="45"/>
+      <c r="Q48" s="45"/>
+      <c r="R48" s="45"/>
+      <c r="S48" s="46"/>
+      <c r="X48" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="Y48" s="44"/>
-      <c r="Z48" s="44"/>
-      <c r="AA48" s="44"/>
-      <c r="AB48" s="44"/>
-      <c r="AC48" s="44"/>
-      <c r="AD48" s="44"/>
-      <c r="AI48" s="44" t="s">
+      <c r="Y48" s="50"/>
+      <c r="Z48" s="50"/>
+      <c r="AA48" s="50"/>
+      <c r="AB48" s="50"/>
+      <c r="AC48" s="50"/>
+      <c r="AD48" s="50"/>
+      <c r="AI48" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="AJ48" s="44"/>
-      <c r="AK48" s="44"/>
-      <c r="AL48" s="44"/>
-      <c r="AM48" s="44"/>
-      <c r="AN48" s="44"/>
-      <c r="AO48" s="44"/>
+      <c r="AJ48" s="50"/>
+      <c r="AK48" s="50"/>
+      <c r="AL48" s="50"/>
+      <c r="AM48" s="50"/>
+      <c r="AN48" s="50"/>
+      <c r="AO48" s="50"/>
     </row>
     <row r="49" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="M48:S48"/>
-    <mergeCell ref="M39:S39"/>
-    <mergeCell ref="P37:V37"/>
-    <mergeCell ref="P28:V28"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="AU45:BA45"/>
+    <mergeCell ref="AF28:AL28"/>
+    <mergeCell ref="AF37:AL37"/>
+    <mergeCell ref="AQ30:AS30"/>
+    <mergeCell ref="AQ41:AS41"/>
+    <mergeCell ref="AU34:BA34"/>
+    <mergeCell ref="AU36:BA36"/>
+    <mergeCell ref="AU2:BA2"/>
+    <mergeCell ref="AU3:BA3"/>
+    <mergeCell ref="AU12:BA12"/>
+    <mergeCell ref="AU14:BA14"/>
+    <mergeCell ref="AU23:BA23"/>
+    <mergeCell ref="X37:AD37"/>
+    <mergeCell ref="AE26:AM26"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="X39:AD39"/>
+    <mergeCell ref="X48:AD48"/>
+    <mergeCell ref="AF1:BA1"/>
+    <mergeCell ref="AI2:AO2"/>
+    <mergeCell ref="AI3:AO3"/>
+    <mergeCell ref="AI12:AO12"/>
+    <mergeCell ref="AI39:AO39"/>
+    <mergeCell ref="AU25:BA25"/>
+    <mergeCell ref="AI48:AO48"/>
+    <mergeCell ref="AN14:AP14"/>
+    <mergeCell ref="AN36:AP36"/>
+    <mergeCell ref="AQ8:AS8"/>
+    <mergeCell ref="AQ19:AS19"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="O26:W26"/>
     <mergeCell ref="I41:K41"/>
@@ -4230,125 +4264,105 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I19:K19"/>
     <mergeCell ref="A25:G25"/>
-    <mergeCell ref="X37:AD37"/>
-    <mergeCell ref="AE26:AM26"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="X39:AD39"/>
-    <mergeCell ref="X48:AD48"/>
-    <mergeCell ref="AF1:BA1"/>
-    <mergeCell ref="AI2:AO2"/>
-    <mergeCell ref="AI3:AO3"/>
-    <mergeCell ref="AI12:AO12"/>
-    <mergeCell ref="AI39:AO39"/>
-    <mergeCell ref="AU25:BA25"/>
-    <mergeCell ref="AI48:AO48"/>
-    <mergeCell ref="AN14:AP14"/>
-    <mergeCell ref="AN36:AP36"/>
-    <mergeCell ref="AQ8:AS8"/>
-    <mergeCell ref="AQ19:AS19"/>
-    <mergeCell ref="AU2:BA2"/>
-    <mergeCell ref="AU3:BA3"/>
-    <mergeCell ref="AU12:BA12"/>
-    <mergeCell ref="AU14:BA14"/>
-    <mergeCell ref="AU23:BA23"/>
-    <mergeCell ref="AU45:BA45"/>
-    <mergeCell ref="AF28:AL28"/>
-    <mergeCell ref="AF37:AL37"/>
-    <mergeCell ref="AQ30:AS30"/>
-    <mergeCell ref="AQ41:AS41"/>
-    <mergeCell ref="AU34:BA34"/>
-    <mergeCell ref="AU36:BA36"/>
+    <mergeCell ref="M48:S48"/>
+    <mergeCell ref="M39:S39"/>
+    <mergeCell ref="P37:V37"/>
+    <mergeCell ref="P28:V28"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="A34:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="15">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$14:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C11 E5:E11 I8:K8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$20:$A$21</xm:f>
           </x14:formula1>
           <xm:sqref>C16:C22 E16:E22 I19:K19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$23:$A$24</xm:f>
           </x14:formula1>
           <xm:sqref>C27:C33 E27:E33 I30:K30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$17:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>C38:C44 E38:E44 I41:K41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>Matchups!$C$14:$C$15</xm:f>
           </x14:formula1>
           <xm:sqref>L14:N14 Q6:Q12 O6:O12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>Matchups!$C$17:$C$18</xm:f>
           </x14:formula1>
           <xm:sqref>L36:N36 Q41:Q47 O41:O47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>Matchups!$E$14:$E$15</xm:f>
           </x14:formula1>
           <xm:sqref>T30:T36 Q30:R36 O26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>Matchups!$F$14:$F$15</xm:f>
           </x14:formula1>
           <xm:sqref>AE26:AM26 AJ30:AJ36 AH30:AH36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>Matchups!$G$13:$G$14</xm:f>
           </x14:formula1>
           <xm:sqref>X37:AD37 Z41:Z47 AB41:AB47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$14:$B$15</xm:f>
           </x14:formula1>
           <xm:sqref>AW5:AW11 AY5:AY11 AQ8:AS8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$20:$B$21</xm:f>
           </x14:formula1>
           <xm:sqref>AW16:AW22 AY16:AY22 AQ19:AS19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$23:$B$24</xm:f>
           </x14:formula1>
           <xm:sqref>AW27:AW33 AY27:AY33 AQ30:AS30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$17:$B$18</xm:f>
           </x14:formula1>
           <xm:sqref>AW38:AW44 AY38:AY44 AQ41:AS41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
           <x14:formula1>
             <xm:f>Matchups!$D$14:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>AN14:AP14 AK5:AK11 AM5:AM11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000E000000}">
           <x14:formula1>
             <xm:f>Matchups!$D$17:$D$18</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Updated Playoff Box Scors, Brackets
Data Input to EOD 5/31/24
</commit_message>
<xml_diff>
--- a/2024/Playoffs/Brackets.xlsx
+++ b/2024/Playoffs/Brackets.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LunchProjects\GitHub\NHLStats\2024\Playoffs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\NHLStats\2024\Playoffs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C10BA9D-6FDF-4C4F-9164-33714821B0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matchups" sheetId="3" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="106">
   <si>
     <t>Eastern Conference Playoff Teams</t>
   </si>
@@ -340,12 +341,15 @@
   </si>
   <si>
     <t>Rangers Lead 2-1</t>
+  </si>
+  <si>
+    <t>Oilers Lead 3-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -718,14 +722,32 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -733,6 +755,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -747,33 +778,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1054,7 +1058,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1147,18 +1151,18 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42" t="s">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42" t="s">
+      <c r="D11" s="44"/>
+      <c r="E11" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="42"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="4" t="s">
         <v>40</v>
       </c>
@@ -1187,18 +1191,18 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="43" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="43" t="s">
+      <c r="D13" s="43"/>
+      <c r="E13" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="44"/>
+      <c r="F13" s="43"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1243,14 +1247,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="43" t="s">
+      <c r="B16" s="43"/>
+      <c r="C16" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="44"/>
+      <c r="D16" s="43"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1281,10 +1285,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="44"/>
+      <c r="B19" s="43"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1303,10 +1307,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="44"/>
+      <c r="B22" s="43"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -1388,16 +1392,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1405,11 +1409,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BB49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC15" workbookViewId="0">
-      <selection activeCell="AI34" sqref="AI34"/>
+    <sheetView tabSelected="1" topLeftCell="K15" workbookViewId="0">
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,124 +1460,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="54"/>
-      <c r="Z1" s="52" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="55"/>
+      <c r="Z1" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="54"/>
-      <c r="AF1" s="52" t="s">
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="55"/>
+      <c r="AF1" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
-      <c r="AW1" s="53"/>
-      <c r="AX1" s="53"/>
-      <c r="AY1" s="53"/>
-      <c r="AZ1" s="53"/>
-      <c r="BA1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
+      <c r="AW1" s="54"/>
+      <c r="AX1" s="54"/>
+      <c r="AY1" s="54"/>
+      <c r="AZ1" s="54"/>
+      <c r="BA1" s="55"/>
     </row>
     <row r="2" spans="1:54" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="50"/>
-      <c r="M2" s="48" t="s">
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59"/>
+      <c r="M2" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="50"/>
-      <c r="AI2" s="48" t="s">
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="59"/>
+      <c r="AI2" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="AJ2" s="49"/>
-      <c r="AK2" s="49"/>
-      <c r="AL2" s="49"/>
-      <c r="AM2" s="49"/>
-      <c r="AN2" s="49"/>
-      <c r="AO2" s="50"/>
-      <c r="AU2" s="48" t="s">
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="58"/>
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="58"/>
+      <c r="AN2" s="58"/>
+      <c r="AO2" s="59"/>
+      <c r="AU2" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="AV2" s="49"/>
-      <c r="AW2" s="49"/>
-      <c r="AX2" s="49"/>
-      <c r="AY2" s="49"/>
-      <c r="AZ2" s="49"/>
-      <c r="BA2" s="50"/>
+      <c r="AV2" s="58"/>
+      <c r="AW2" s="58"/>
+      <c r="AX2" s="58"/>
+      <c r="AY2" s="58"/>
+      <c r="AZ2" s="58"/>
+      <c r="BA2" s="59"/>
     </row>
     <row r="3" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="AI3" s="45" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="AI3" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="AJ3" s="45"/>
-      <c r="AK3" s="45"/>
-      <c r="AL3" s="45"/>
-      <c r="AM3" s="45"/>
-      <c r="AN3" s="45"/>
-      <c r="AO3" s="45"/>
-      <c r="AU3" s="45" t="s">
+      <c r="AJ3" s="51"/>
+      <c r="AK3" s="51"/>
+      <c r="AL3" s="51"/>
+      <c r="AM3" s="51"/>
+      <c r="AN3" s="51"/>
+      <c r="AO3" s="51"/>
+      <c r="AU3" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AV3" s="45"/>
-      <c r="AW3" s="45"/>
-      <c r="AX3" s="45"/>
-      <c r="AY3" s="45"/>
-      <c r="AZ3" s="45"/>
-      <c r="BA3" s="45"/>
+      <c r="AV3" s="51"/>
+      <c r="AW3" s="51"/>
+      <c r="AX3" s="51"/>
+      <c r="AY3" s="51"/>
+      <c r="AZ3" s="51"/>
+      <c r="BA3" s="51"/>
     </row>
     <row r="4" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -1597,15 +1601,15 @@
       <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="55" t="s">
+      <c r="M4" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="57"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="47"/>
       <c r="AI4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1935,11 +1939,11 @@
       <c r="G8" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="I8" s="46" t="s">
+      <c r="I8" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
       <c r="M8" s="8">
         <v>3</v>
       </c>
@@ -1985,11 +1989,11 @@
       <c r="AO8" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="AQ8" s="46" t="s">
+      <c r="AQ8" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="AR8" s="46"/>
-      <c r="AS8" s="46"/>
+      <c r="AR8" s="52"/>
+      <c r="AS8" s="52"/>
       <c r="AU8" s="38">
         <v>4</v>
       </c>
@@ -2250,15 +2254,15 @@
       <c r="BA11" s="6"/>
     </row>
     <row r="12" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
       <c r="L12" s="12"/>
       <c r="M12" s="8" t="s">
         <v>28</v>
@@ -2273,69 +2277,69 @@
       </c>
       <c r="R12" s="13"/>
       <c r="S12" s="16"/>
-      <c r="AI12" s="45" t="s">
+      <c r="AI12" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="AJ12" s="45"/>
-      <c r="AK12" s="45"/>
-      <c r="AL12" s="45"/>
-      <c r="AM12" s="45"/>
-      <c r="AN12" s="45"/>
-      <c r="AO12" s="45"/>
+      <c r="AJ12" s="51"/>
+      <c r="AK12" s="51"/>
+      <c r="AL12" s="51"/>
+      <c r="AM12" s="51"/>
+      <c r="AN12" s="51"/>
+      <c r="AO12" s="51"/>
       <c r="AQ12" s="12"/>
-      <c r="AU12" s="45" t="s">
+      <c r="AU12" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="AV12" s="45"/>
-      <c r="AW12" s="45"/>
-      <c r="AX12" s="45"/>
-      <c r="AY12" s="45"/>
-      <c r="AZ12" s="45"/>
-      <c r="BA12" s="45"/>
+      <c r="AV12" s="51"/>
+      <c r="AW12" s="51"/>
+      <c r="AX12" s="51"/>
+      <c r="AY12" s="51"/>
+      <c r="AZ12" s="51"/>
+      <c r="BA12" s="51"/>
     </row>
     <row r="13" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L13" s="12"/>
-      <c r="M13" s="55" t="s">
+      <c r="M13" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="56"/>
-      <c r="O13" s="56"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="56"/>
-      <c r="S13" s="57"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="46"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="46"/>
+      <c r="S13" s="47"/>
       <c r="AQ13" s="12"/>
     </row>
     <row r="14" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="L14" s="47" t="s">
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="L14" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="M14" s="46"/>
-      <c r="N14" s="46"/>
-      <c r="AN14" s="46" t="s">
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="AN14" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="AO14" s="46"/>
-      <c r="AP14" s="46"/>
+      <c r="AO14" s="52"/>
+      <c r="AP14" s="52"/>
       <c r="AQ14" s="12"/>
-      <c r="AU14" s="45" t="s">
+      <c r="AU14" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AV14" s="45"/>
-      <c r="AW14" s="45"/>
-      <c r="AX14" s="45"/>
-      <c r="AY14" s="45"/>
-      <c r="AZ14" s="45"/>
-      <c r="BA14" s="45"/>
+      <c r="AV14" s="51"/>
+      <c r="AW14" s="51"/>
+      <c r="AX14" s="51"/>
+      <c r="AY14" s="51"/>
+      <c r="AZ14" s="51"/>
+      <c r="BA14" s="51"/>
     </row>
     <row r="15" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -2557,19 +2561,19 @@
       <c r="H19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
+      <c r="I19" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
       <c r="L19" s="12"/>
       <c r="O19" s="12"/>
       <c r="AN19" s="12"/>
-      <c r="AQ19" s="47" t="s">
+      <c r="AQ19" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="AR19" s="46"/>
-      <c r="AS19" s="46"/>
+      <c r="AR19" s="52"/>
+      <c r="AS19" s="52"/>
       <c r="AU19" s="38">
         <v>4</v>
       </c>
@@ -2699,52 +2703,52 @@
       <c r="BA22" s="6"/>
     </row>
     <row r="23" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
       <c r="O23" s="12"/>
       <c r="AN23" s="12"/>
-      <c r="AU23" s="45" t="s">
+      <c r="AU23" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="AV23" s="45"/>
-      <c r="AW23" s="45"/>
-      <c r="AX23" s="45"/>
-      <c r="AY23" s="45"/>
-      <c r="AZ23" s="45"/>
-      <c r="BA23" s="45"/>
+      <c r="AV23" s="51"/>
+      <c r="AW23" s="51"/>
+      <c r="AX23" s="51"/>
+      <c r="AY23" s="51"/>
+      <c r="AZ23" s="51"/>
+      <c r="BA23" s="51"/>
     </row>
     <row r="24" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O24" s="12"/>
       <c r="AN24" s="12"/>
     </row>
     <row r="25" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
       <c r="O25" s="12"/>
       <c r="AN25" s="12"/>
-      <c r="AU25" s="45" t="s">
+      <c r="AU25" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="AV25" s="45"/>
-      <c r="AW25" s="45"/>
-      <c r="AX25" s="45"/>
-      <c r="AY25" s="45"/>
-      <c r="AZ25" s="45"/>
-      <c r="BA25" s="45"/>
+      <c r="AV25" s="51"/>
+      <c r="AW25" s="51"/>
+      <c r="AX25" s="51"/>
+      <c r="AY25" s="51"/>
+      <c r="AZ25" s="51"/>
+      <c r="BA25" s="51"/>
     </row>
     <row r="26" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="20" t="s">
@@ -2768,24 +2772,24 @@
       <c r="G26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="O26" s="47"/>
-      <c r="P26" s="46"/>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="46"/>
-      <c r="S26" s="46"/>
-      <c r="T26" s="46"/>
-      <c r="U26" s="46"/>
-      <c r="V26" s="46"/>
-      <c r="W26" s="46"/>
-      <c r="AE26" s="46"/>
-      <c r="AF26" s="46"/>
-      <c r="AG26" s="46"/>
-      <c r="AH26" s="46"/>
-      <c r="AI26" s="46"/>
-      <c r="AJ26" s="46"/>
-      <c r="AK26" s="46"/>
-      <c r="AL26" s="46"/>
-      <c r="AM26" s="51"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="52"/>
+      <c r="Q26" s="52"/>
+      <c r="R26" s="52"/>
+      <c r="S26" s="52"/>
+      <c r="T26" s="52"/>
+      <c r="U26" s="52"/>
+      <c r="V26" s="52"/>
+      <c r="W26" s="52"/>
+      <c r="AE26" s="52"/>
+      <c r="AF26" s="52"/>
+      <c r="AG26" s="52"/>
+      <c r="AH26" s="52"/>
+      <c r="AI26" s="52"/>
+      <c r="AJ26" s="52"/>
+      <c r="AK26" s="52"/>
+      <c r="AL26" s="52"/>
+      <c r="AM26" s="60"/>
       <c r="AU26" s="20" t="s">
         <v>18</v>
       </c>
@@ -2879,26 +2883,26 @@
         <v>56</v>
       </c>
       <c r="O28" s="12"/>
-      <c r="P28" s="55" t="s">
+      <c r="P28" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="56"/>
-      <c r="S28" s="56"/>
-      <c r="T28" s="56"/>
-      <c r="U28" s="56"/>
-      <c r="V28" s="57"/>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="46"/>
+      <c r="S28" s="46"/>
+      <c r="T28" s="46"/>
+      <c r="U28" s="46"/>
+      <c r="V28" s="47"/>
       <c r="X28" s="12"/>
       <c r="AD28" s="13"/>
-      <c r="AF28" s="45" t="s">
+      <c r="AF28" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="AG28" s="45"/>
-      <c r="AH28" s="45"/>
-      <c r="AI28" s="45"/>
-      <c r="AJ28" s="45"/>
-      <c r="AK28" s="45"/>
-      <c r="AL28" s="45"/>
+      <c r="AG28" s="51"/>
+      <c r="AH28" s="51"/>
+      <c r="AI28" s="51"/>
+      <c r="AJ28" s="51"/>
+      <c r="AK28" s="51"/>
+      <c r="AL28" s="51"/>
       <c r="AN28" s="12"/>
       <c r="AU28" s="8">
         <v>2</v>
@@ -3034,11 +3038,11 @@
       <c r="G30" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="I30" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
+      <c r="I30" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="J30" s="52"/>
+      <c r="K30" s="52"/>
       <c r="O30" s="12"/>
       <c r="P30" s="7">
         <v>1</v>
@@ -3088,11 +3092,11 @@
         <v>79</v>
       </c>
       <c r="AN30" s="12"/>
-      <c r="AQ30" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="AR30" s="46"/>
-      <c r="AS30" s="46"/>
+      <c r="AQ30" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR30" s="52"/>
+      <c r="AS30" s="52"/>
       <c r="AU30" s="38">
         <v>4</v>
       </c>
@@ -3387,15 +3391,15 @@
       <c r="BA33" s="6"/>
     </row>
     <row r="34" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="45" t="s">
+      <c r="A34" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="45"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
       <c r="L34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="8" t="s">
@@ -3425,28 +3429,34 @@
         <v>27</v>
       </c>
       <c r="AG34" s="27">
-        <v>45444</v>
+        <v>45443</v>
       </c>
       <c r="AH34" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="AI34" s="13"/>
+      <c r="AI34" s="13">
+        <v>3</v>
+      </c>
       <c r="AJ34" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AK34" s="13"/>
-      <c r="AL34" s="16"/>
+      <c r="AK34" s="13">
+        <v>1</v>
+      </c>
+      <c r="AL34" s="16" t="s">
+        <v>105</v>
+      </c>
       <c r="AN34" s="12"/>
       <c r="AQ34" s="12"/>
-      <c r="AU34" s="45" t="s">
+      <c r="AU34" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="AV34" s="45"/>
-      <c r="AW34" s="45"/>
-      <c r="AX34" s="45"/>
-      <c r="AY34" s="45"/>
-      <c r="AZ34" s="45"/>
-      <c r="BA34" s="45"/>
+      <c r="AV34" s="51"/>
+      <c r="AW34" s="51"/>
+      <c r="AX34" s="51"/>
+      <c r="AY34" s="51"/>
+      <c r="AZ34" s="51"/>
+      <c r="BA34" s="51"/>
     </row>
     <row r="35" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L35" s="12"/>
@@ -3471,7 +3481,9 @@
       <c r="AF35" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AG35" s="27"/>
+      <c r="AG35" s="27">
+        <v>45445</v>
+      </c>
       <c r="AH35" s="12" t="s">
         <v>5</v>
       </c>
@@ -3485,20 +3497,20 @@
       <c r="AQ35" s="12"/>
     </row>
     <row r="36" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="L36" s="47" t="s">
+      <c r="B36" s="51"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="L36" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="M36" s="46"/>
-      <c r="N36" s="46"/>
+      <c r="M36" s="52"/>
+      <c r="N36" s="52"/>
       <c r="O36" s="12"/>
       <c r="P36" s="8" t="s">
         <v>28</v>
@@ -3528,21 +3540,21 @@
       </c>
       <c r="AK36" s="36"/>
       <c r="AL36" s="37"/>
-      <c r="AN36" s="47" t="s">
+      <c r="AN36" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="AO36" s="46"/>
-      <c r="AP36" s="46"/>
+      <c r="AO36" s="52"/>
+      <c r="AP36" s="52"/>
       <c r="AQ36" s="12"/>
-      <c r="AU36" s="45" t="s">
+      <c r="AU36" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="AV36" s="45"/>
-      <c r="AW36" s="45"/>
-      <c r="AX36" s="45"/>
-      <c r="AY36" s="45"/>
-      <c r="AZ36" s="45"/>
-      <c r="BA36" s="45"/>
+      <c r="AV36" s="51"/>
+      <c r="AW36" s="51"/>
+      <c r="AX36" s="51"/>
+      <c r="AY36" s="51"/>
+      <c r="AZ36" s="51"/>
+      <c r="BA36" s="51"/>
     </row>
     <row r="37" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="20" t="s">
@@ -3567,31 +3579,31 @@
         <v>25</v>
       </c>
       <c r="L37" s="12"/>
-      <c r="P37" s="58" t="s">
+      <c r="P37" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="Q37" s="59"/>
-      <c r="R37" s="59"/>
-      <c r="S37" s="59"/>
-      <c r="T37" s="59"/>
-      <c r="U37" s="59"/>
-      <c r="V37" s="60"/>
-      <c r="X37" s="47"/>
-      <c r="Y37" s="46"/>
-      <c r="Z37" s="46"/>
-      <c r="AA37" s="46"/>
-      <c r="AB37" s="46"/>
-      <c r="AC37" s="46"/>
-      <c r="AD37" s="51"/>
-      <c r="AF37" s="45" t="s">
+      <c r="Q37" s="49"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="49"/>
+      <c r="T37" s="49"/>
+      <c r="U37" s="49"/>
+      <c r="V37" s="50"/>
+      <c r="X37" s="56"/>
+      <c r="Y37" s="52"/>
+      <c r="Z37" s="52"/>
+      <c r="AA37" s="52"/>
+      <c r="AB37" s="52"/>
+      <c r="AC37" s="52"/>
+      <c r="AD37" s="60"/>
+      <c r="AF37" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="AG37" s="45"/>
-      <c r="AH37" s="45"/>
-      <c r="AI37" s="45"/>
-      <c r="AJ37" s="45"/>
-      <c r="AK37" s="45"/>
-      <c r="AL37" s="45"/>
+      <c r="AG37" s="51"/>
+      <c r="AH37" s="51"/>
+      <c r="AI37" s="51"/>
+      <c r="AJ37" s="51"/>
+      <c r="AK37" s="51"/>
+      <c r="AL37" s="51"/>
       <c r="AQ37" s="12"/>
       <c r="AU37" s="3" t="s">
         <v>18</v>
@@ -3687,33 +3699,33 @@
         <v>59</v>
       </c>
       <c r="L39" s="12"/>
-      <c r="M39" s="55" t="s">
+      <c r="M39" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="N39" s="56"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="56"/>
-      <c r="Q39" s="56"/>
-      <c r="R39" s="56"/>
-      <c r="S39" s="57"/>
-      <c r="X39" s="45" t="s">
+      <c r="N39" s="46"/>
+      <c r="O39" s="46"/>
+      <c r="P39" s="46"/>
+      <c r="Q39" s="46"/>
+      <c r="R39" s="46"/>
+      <c r="S39" s="47"/>
+      <c r="X39" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="Y39" s="45"/>
-      <c r="Z39" s="45"/>
-      <c r="AA39" s="45"/>
-      <c r="AB39" s="45"/>
-      <c r="AC39" s="45"/>
-      <c r="AD39" s="45"/>
-      <c r="AI39" s="45" t="s">
+      <c r="Y39" s="51"/>
+      <c r="Z39" s="51"/>
+      <c r="AA39" s="51"/>
+      <c r="AB39" s="51"/>
+      <c r="AC39" s="51"/>
+      <c r="AD39" s="51"/>
+      <c r="AI39" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="AJ39" s="45"/>
-      <c r="AK39" s="45"/>
-      <c r="AL39" s="45"/>
-      <c r="AM39" s="45"/>
-      <c r="AN39" s="45"/>
-      <c r="AO39" s="45"/>
+      <c r="AJ39" s="51"/>
+      <c r="AK39" s="51"/>
+      <c r="AL39" s="51"/>
+      <c r="AM39" s="51"/>
+      <c r="AN39" s="51"/>
+      <c r="AO39" s="51"/>
       <c r="AQ39" s="12"/>
       <c r="AU39" s="8">
         <v>2</v>
@@ -3871,11 +3883,11 @@
       <c r="G41" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="I41" s="46" t="s">
+      <c r="I41" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="J41" s="46"/>
-      <c r="K41" s="46"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="52"/>
       <c r="L41" s="12"/>
       <c r="M41" s="7">
         <v>1</v>
@@ -3931,11 +3943,11 @@
       <c r="AP41" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AQ41" s="47" t="s">
+      <c r="AQ41" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="AR41" s="46"/>
-      <c r="AS41" s="46"/>
+      <c r="AR41" s="52"/>
+      <c r="AS41" s="52"/>
       <c r="AU41" s="8">
         <v>4</v>
       </c>
@@ -4228,15 +4240,15 @@
       </c>
     </row>
     <row r="45" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="45" t="s">
+      <c r="A45" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
       <c r="M45" s="8" t="s">
         <v>27</v>
       </c>
@@ -4288,15 +4300,15 @@
       <c r="AO45" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="AU45" s="45" t="s">
+      <c r="AU45" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="AV45" s="45"/>
-      <c r="AW45" s="45"/>
-      <c r="AX45" s="45"/>
-      <c r="AY45" s="45"/>
-      <c r="AZ45" s="45"/>
-      <c r="BA45" s="45"/>
+      <c r="AV45" s="51"/>
+      <c r="AW45" s="51"/>
+      <c r="AX45" s="51"/>
+      <c r="AY45" s="51"/>
+      <c r="AZ45" s="51"/>
+      <c r="BA45" s="51"/>
     </row>
     <row r="46" spans="1:54" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="M46" s="8" t="s">
@@ -4392,45 +4404,65 @@
       <c r="AO47" s="6"/>
     </row>
     <row r="48" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M48" s="55" t="s">
+      <c r="M48" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="N48" s="56"/>
-      <c r="O48" s="56"/>
-      <c r="P48" s="56"/>
-      <c r="Q48" s="56"/>
-      <c r="R48" s="56"/>
-      <c r="S48" s="57"/>
-      <c r="X48" s="45" t="s">
+      <c r="N48" s="46"/>
+      <c r="O48" s="46"/>
+      <c r="P48" s="46"/>
+      <c r="Q48" s="46"/>
+      <c r="R48" s="46"/>
+      <c r="S48" s="47"/>
+      <c r="X48" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="Y48" s="45"/>
-      <c r="Z48" s="45"/>
-      <c r="AA48" s="45"/>
-      <c r="AB48" s="45"/>
-      <c r="AC48" s="45"/>
-      <c r="AD48" s="45"/>
-      <c r="AI48" s="45" t="s">
+      <c r="Y48" s="51"/>
+      <c r="Z48" s="51"/>
+      <c r="AA48" s="51"/>
+      <c r="AB48" s="51"/>
+      <c r="AC48" s="51"/>
+      <c r="AD48" s="51"/>
+      <c r="AI48" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="AJ48" s="45"/>
-      <c r="AK48" s="45"/>
-      <c r="AL48" s="45"/>
-      <c r="AM48" s="45"/>
-      <c r="AN48" s="45"/>
-      <c r="AO48" s="45"/>
+      <c r="AJ48" s="51"/>
+      <c r="AK48" s="51"/>
+      <c r="AL48" s="51"/>
+      <c r="AM48" s="51"/>
+      <c r="AN48" s="51"/>
+      <c r="AO48" s="51"/>
     </row>
     <row r="49" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="M48:S48"/>
-    <mergeCell ref="M39:S39"/>
-    <mergeCell ref="P37:V37"/>
-    <mergeCell ref="P28:V28"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="AU45:BA45"/>
+    <mergeCell ref="AF28:AL28"/>
+    <mergeCell ref="AF37:AL37"/>
+    <mergeCell ref="AQ30:AS30"/>
+    <mergeCell ref="AQ41:AS41"/>
+    <mergeCell ref="AU34:BA34"/>
+    <mergeCell ref="AU36:BA36"/>
+    <mergeCell ref="AU2:BA2"/>
+    <mergeCell ref="AU3:BA3"/>
+    <mergeCell ref="AU12:BA12"/>
+    <mergeCell ref="AU14:BA14"/>
+    <mergeCell ref="AU23:BA23"/>
+    <mergeCell ref="X37:AD37"/>
+    <mergeCell ref="AE26:AM26"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="X39:AD39"/>
+    <mergeCell ref="X48:AD48"/>
+    <mergeCell ref="AF1:BA1"/>
+    <mergeCell ref="AI2:AO2"/>
+    <mergeCell ref="AI3:AO3"/>
+    <mergeCell ref="AI12:AO12"/>
+    <mergeCell ref="AI39:AO39"/>
+    <mergeCell ref="AU25:BA25"/>
+    <mergeCell ref="AI48:AO48"/>
+    <mergeCell ref="AN14:AP14"/>
+    <mergeCell ref="AN36:AP36"/>
+    <mergeCell ref="AQ8:AS8"/>
+    <mergeCell ref="AQ19:AS19"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="O26:W26"/>
     <mergeCell ref="I41:K41"/>
@@ -4447,125 +4479,105 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I19:K19"/>
     <mergeCell ref="A25:G25"/>
-    <mergeCell ref="X37:AD37"/>
-    <mergeCell ref="AE26:AM26"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="X39:AD39"/>
-    <mergeCell ref="X48:AD48"/>
-    <mergeCell ref="AF1:BA1"/>
-    <mergeCell ref="AI2:AO2"/>
-    <mergeCell ref="AI3:AO3"/>
-    <mergeCell ref="AI12:AO12"/>
-    <mergeCell ref="AI39:AO39"/>
-    <mergeCell ref="AU25:BA25"/>
-    <mergeCell ref="AI48:AO48"/>
-    <mergeCell ref="AN14:AP14"/>
-    <mergeCell ref="AN36:AP36"/>
-    <mergeCell ref="AQ8:AS8"/>
-    <mergeCell ref="AQ19:AS19"/>
-    <mergeCell ref="AU2:BA2"/>
-    <mergeCell ref="AU3:BA3"/>
-    <mergeCell ref="AU12:BA12"/>
-    <mergeCell ref="AU14:BA14"/>
-    <mergeCell ref="AU23:BA23"/>
-    <mergeCell ref="AU45:BA45"/>
-    <mergeCell ref="AF28:AL28"/>
-    <mergeCell ref="AF37:AL37"/>
-    <mergeCell ref="AQ30:AS30"/>
-    <mergeCell ref="AQ41:AS41"/>
-    <mergeCell ref="AU34:BA34"/>
-    <mergeCell ref="AU36:BA36"/>
+    <mergeCell ref="M48:S48"/>
+    <mergeCell ref="M39:S39"/>
+    <mergeCell ref="P37:V37"/>
+    <mergeCell ref="P28:V28"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="A34:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="15">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$14:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C11 E5:E11 I8:K8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$20:$A$21</xm:f>
           </x14:formula1>
           <xm:sqref>C16:C22 E16:E22 I19:K19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$23:$A$24</xm:f>
           </x14:formula1>
           <xm:sqref>C27:C33 E27:E33 I30:K30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>Matchups!$A$17:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>C38:C44 E38:E44 I41:K41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>Matchups!$C$14:$C$15</xm:f>
           </x14:formula1>
           <xm:sqref>L14:N14 Q6:Q12 O6:O12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>Matchups!$C$17:$C$18</xm:f>
           </x14:formula1>
           <xm:sqref>L36:N36 Q41:Q47 O41:O47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>Matchups!$E$14:$E$15</xm:f>
           </x14:formula1>
           <xm:sqref>T30:T36 O26 R30:R36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>Matchups!$F$14:$F$15</xm:f>
           </x14:formula1>
           <xm:sqref>AE26:AM26 AJ30:AJ36 AH30:AH36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>Matchups!$G$13:$G$14</xm:f>
           </x14:formula1>
           <xm:sqref>X37:AD37 Z41:Z47 AB41:AB47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$14:$B$15</xm:f>
           </x14:formula1>
           <xm:sqref>AW5:AW11 AY5:AY11 AQ8:AS8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$20:$B$21</xm:f>
           </x14:formula1>
           <xm:sqref>AW16:AW22 AY16:AY22 AQ19:AS19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$23:$B$24</xm:f>
           </x14:formula1>
           <xm:sqref>AW27:AW33 AY27:AY33 AQ30:AS30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
           <x14:formula1>
             <xm:f>Matchups!$B$17:$B$18</xm:f>
           </x14:formula1>
           <xm:sqref>AW38:AW44 AY38:AY44 AQ41:AS41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
           <x14:formula1>
             <xm:f>Matchups!$D$14:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>AN14:AP14 AK5:AK11 AM5:AM11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000E000000}">
           <x14:formula1>
             <xm:f>Matchups!$D$17:$D$18</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Updated Playoff Box Scores Brackets
Completed season.
</commit_message>
<xml_diff>
--- a/2024/Playoffs/Brackets.xlsx
+++ b/2024/Playoffs/Brackets.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\NHLStats\2024\Playoffs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LunchProjects\GitHub\NHLStats\2024\Playoffs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF2E433-7079-4731-83AA-24C9CE990D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Matchups" sheetId="3" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="108">
   <si>
     <t>Eastern Conference Playoff Teams</t>
   </si>
@@ -347,12 +346,15 @@
   </si>
   <si>
     <t>Oilers Win Series 4-2</t>
+  </si>
+  <si>
+    <t>Panthers Win Series 4-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -725,13 +727,43 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -751,36 +783,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1061,7 +1063,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1154,18 +1156,18 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44" t="s">
+      <c r="D11" s="42"/>
+      <c r="E11" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="44"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="4" t="s">
         <v>40</v>
       </c>
@@ -1194,18 +1196,18 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="42" t="s">
+      <c r="B13" s="44"/>
+      <c r="C13" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="42" t="s">
+      <c r="D13" s="44"/>
+      <c r="E13" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="43"/>
+      <c r="F13" s="44"/>
       <c r="G13" s="5" t="s">
         <v>6</v>
       </c>
@@ -1254,14 +1256,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="42" t="s">
+      <c r="B16" s="44"/>
+      <c r="C16" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="43"/>
+      <c r="D16" s="44"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1292,10 +1294,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="43"/>
+      <c r="B19" s="44"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1314,10 +1316,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="43"/>
+      <c r="B22" s="44"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -1399,16 +1401,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1416,7 +1418,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R25" workbookViewId="0">
@@ -1446,7 +1448,7 @@
     <col min="24" max="24" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="28" width="21.42578125" style="1" customWidth="1"/>
     <col min="29" max="29" width="9.140625" style="1"/>
-    <col min="30" max="30" width="20.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="32" width="9.140625" style="1"/>
     <col min="33" max="33" width="23.7109375" style="1" customWidth="1"/>
     <col min="34" max="34" width="22.85546875" style="1" customWidth="1"/>
@@ -1467,124 +1469,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="55"/>
-      <c r="Z1" s="53" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="54"/>
+      <c r="Z1" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="55"/>
-      <c r="AF1" s="53" t="s">
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="54"/>
+      <c r="AF1" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
-      <c r="AW1" s="54"/>
-      <c r="AX1" s="54"/>
-      <c r="AY1" s="54"/>
-      <c r="AZ1" s="54"/>
-      <c r="BA1" s="55"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="53"/>
+      <c r="AL1" s="53"/>
+      <c r="AM1" s="53"/>
+      <c r="AN1" s="53"/>
+      <c r="AO1" s="53"/>
+      <c r="AP1" s="53"/>
+      <c r="AQ1" s="53"/>
+      <c r="AR1" s="53"/>
+      <c r="AS1" s="53"/>
+      <c r="AT1" s="53"/>
+      <c r="AU1" s="53"/>
+      <c r="AV1" s="53"/>
+      <c r="AW1" s="53"/>
+      <c r="AX1" s="53"/>
+      <c r="AY1" s="53"/>
+      <c r="AZ1" s="53"/>
+      <c r="BA1" s="54"/>
     </row>
     <row r="2" spans="1:54" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="59"/>
-      <c r="M2" s="57" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="M2" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="59"/>
-      <c r="AI2" s="57" t="s">
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="50"/>
+      <c r="AI2" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="AJ2" s="58"/>
-      <c r="AK2" s="58"/>
-      <c r="AL2" s="58"/>
-      <c r="AM2" s="58"/>
-      <c r="AN2" s="58"/>
-      <c r="AO2" s="59"/>
-      <c r="AU2" s="57" t="s">
+      <c r="AJ2" s="49"/>
+      <c r="AK2" s="49"/>
+      <c r="AL2" s="49"/>
+      <c r="AM2" s="49"/>
+      <c r="AN2" s="49"/>
+      <c r="AO2" s="50"/>
+      <c r="AU2" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="AV2" s="58"/>
-      <c r="AW2" s="58"/>
-      <c r="AX2" s="58"/>
-      <c r="AY2" s="58"/>
-      <c r="AZ2" s="58"/>
-      <c r="BA2" s="59"/>
+      <c r="AV2" s="49"/>
+      <c r="AW2" s="49"/>
+      <c r="AX2" s="49"/>
+      <c r="AY2" s="49"/>
+      <c r="AZ2" s="49"/>
+      <c r="BA2" s="50"/>
     </row>
     <row r="3" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="AI3" s="51" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="AI3" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="51"/>
-      <c r="AL3" s="51"/>
-      <c r="AM3" s="51"/>
-      <c r="AN3" s="51"/>
-      <c r="AO3" s="51"/>
-      <c r="AU3" s="51" t="s">
+      <c r="AJ3" s="45"/>
+      <c r="AK3" s="45"/>
+      <c r="AL3" s="45"/>
+      <c r="AM3" s="45"/>
+      <c r="AN3" s="45"/>
+      <c r="AO3" s="45"/>
+      <c r="AU3" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="AV3" s="51"/>
-      <c r="AW3" s="51"/>
-      <c r="AX3" s="51"/>
-      <c r="AY3" s="51"/>
-      <c r="AZ3" s="51"/>
-      <c r="BA3" s="51"/>
+      <c r="AV3" s="45"/>
+      <c r="AW3" s="45"/>
+      <c r="AX3" s="45"/>
+      <c r="AY3" s="45"/>
+      <c r="AZ3" s="45"/>
+      <c r="BA3" s="45"/>
     </row>
     <row r="4" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -1608,15 +1610,15 @@
       <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="M4" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="47"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="57"/>
       <c r="AI4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1946,11 +1948,11 @@
       <c r="G8" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="I8" s="52" t="s">
+      <c r="I8" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
       <c r="M8" s="8">
         <v>3</v>
       </c>
@@ -1996,11 +1998,11 @@
       <c r="AO8" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="AQ8" s="52" t="s">
+      <c r="AQ8" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="AR8" s="52"/>
-      <c r="AS8" s="52"/>
+      <c r="AR8" s="46"/>
+      <c r="AS8" s="46"/>
       <c r="AU8" s="38">
         <v>4</v>
       </c>
@@ -2261,15 +2263,15 @@
       <c r="BA11" s="6"/>
     </row>
     <row r="12" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
       <c r="L12" s="12"/>
       <c r="M12" s="8" t="s">
         <v>28</v>
@@ -2284,69 +2286,69 @@
       </c>
       <c r="R12" s="13"/>
       <c r="S12" s="16"/>
-      <c r="AI12" s="51" t="s">
+      <c r="AI12" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="AJ12" s="51"/>
-      <c r="AK12" s="51"/>
-      <c r="AL12" s="51"/>
-      <c r="AM12" s="51"/>
-      <c r="AN12" s="51"/>
-      <c r="AO12" s="51"/>
+      <c r="AJ12" s="45"/>
+      <c r="AK12" s="45"/>
+      <c r="AL12" s="45"/>
+      <c r="AM12" s="45"/>
+      <c r="AN12" s="45"/>
+      <c r="AO12" s="45"/>
       <c r="AQ12" s="12"/>
-      <c r="AU12" s="51" t="s">
+      <c r="AU12" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="AV12" s="51"/>
-      <c r="AW12" s="51"/>
-      <c r="AX12" s="51"/>
-      <c r="AY12" s="51"/>
-      <c r="AZ12" s="51"/>
-      <c r="BA12" s="51"/>
+      <c r="AV12" s="45"/>
+      <c r="AW12" s="45"/>
+      <c r="AX12" s="45"/>
+      <c r="AY12" s="45"/>
+      <c r="AZ12" s="45"/>
+      <c r="BA12" s="45"/>
     </row>
     <row r="13" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L13" s="12"/>
-      <c r="M13" s="45" t="s">
+      <c r="M13" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="47"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="56"/>
+      <c r="R13" s="56"/>
+      <c r="S13" s="57"/>
       <c r="AQ13" s="12"/>
     </row>
     <row r="14" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="L14" s="56" t="s">
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="L14" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="AN14" s="52" t="s">
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
+      <c r="AN14" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="AO14" s="52"/>
-      <c r="AP14" s="52"/>
+      <c r="AO14" s="46"/>
+      <c r="AP14" s="46"/>
       <c r="AQ14" s="12"/>
-      <c r="AU14" s="51" t="s">
+      <c r="AU14" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="AV14" s="51"/>
-      <c r="AW14" s="51"/>
-      <c r="AX14" s="51"/>
-      <c r="AY14" s="51"/>
-      <c r="AZ14" s="51"/>
-      <c r="BA14" s="51"/>
+      <c r="AV14" s="45"/>
+      <c r="AW14" s="45"/>
+      <c r="AX14" s="45"/>
+      <c r="AY14" s="45"/>
+      <c r="AZ14" s="45"/>
+      <c r="BA14" s="45"/>
     </row>
     <row r="15" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -2568,19 +2570,19 @@
       <c r="H19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
+      <c r="I19" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
       <c r="L19" s="12"/>
       <c r="O19" s="12"/>
       <c r="AN19" s="12"/>
-      <c r="AQ19" s="56" t="s">
+      <c r="AQ19" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="AR19" s="52"/>
-      <c r="AS19" s="52"/>
+      <c r="AR19" s="46"/>
+      <c r="AS19" s="46"/>
       <c r="AU19" s="38">
         <v>4</v>
       </c>
@@ -2710,52 +2712,52 @@
       <c r="BA22" s="6"/>
     </row>
     <row r="23" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
       <c r="O23" s="12"/>
       <c r="AN23" s="12"/>
-      <c r="AU23" s="51" t="s">
+      <c r="AU23" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="AV23" s="51"/>
-      <c r="AW23" s="51"/>
-      <c r="AX23" s="51"/>
-      <c r="AY23" s="51"/>
-      <c r="AZ23" s="51"/>
-      <c r="BA23" s="51"/>
+      <c r="AV23" s="45"/>
+      <c r="AW23" s="45"/>
+      <c r="AX23" s="45"/>
+      <c r="AY23" s="45"/>
+      <c r="AZ23" s="45"/>
+      <c r="BA23" s="45"/>
     </row>
     <row r="24" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O24" s="12"/>
       <c r="AN24" s="12"/>
     </row>
     <row r="25" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
       <c r="O25" s="12"/>
       <c r="AN25" s="12"/>
-      <c r="AU25" s="51" t="s">
+      <c r="AU25" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="AV25" s="51"/>
-      <c r="AW25" s="51"/>
-      <c r="AX25" s="51"/>
-      <c r="AY25" s="51"/>
-      <c r="AZ25" s="51"/>
-      <c r="BA25" s="51"/>
+      <c r="AV25" s="45"/>
+      <c r="AW25" s="45"/>
+      <c r="AX25" s="45"/>
+      <c r="AY25" s="45"/>
+      <c r="AZ25" s="45"/>
+      <c r="BA25" s="45"/>
     </row>
     <row r="26" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="20" t="s">
@@ -2779,28 +2781,28 @@
       <c r="G26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="O26" s="56" t="s">
+      <c r="O26" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="P26" s="52"/>
-      <c r="Q26" s="52"/>
-      <c r="R26" s="52"/>
-      <c r="S26" s="52"/>
-      <c r="T26" s="52"/>
-      <c r="U26" s="52"/>
-      <c r="V26" s="52"/>
-      <c r="W26" s="52"/>
-      <c r="AE26" s="52" t="s">
+      <c r="P26" s="46"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="46"/>
+      <c r="S26" s="46"/>
+      <c r="T26" s="46"/>
+      <c r="U26" s="46"/>
+      <c r="V26" s="46"/>
+      <c r="W26" s="46"/>
+      <c r="AE26" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="AF26" s="52"/>
-      <c r="AG26" s="52"/>
-      <c r="AH26" s="52"/>
-      <c r="AI26" s="52"/>
-      <c r="AJ26" s="52"/>
-      <c r="AK26" s="52"/>
-      <c r="AL26" s="52"/>
-      <c r="AM26" s="60"/>
+      <c r="AF26" s="46"/>
+      <c r="AG26" s="46"/>
+      <c r="AH26" s="46"/>
+      <c r="AI26" s="46"/>
+      <c r="AJ26" s="46"/>
+      <c r="AK26" s="46"/>
+      <c r="AL26" s="46"/>
+      <c r="AM26" s="51"/>
       <c r="AU26" s="20" t="s">
         <v>18</v>
       </c>
@@ -2894,26 +2896,26 @@
         <v>56</v>
       </c>
       <c r="O28" s="12"/>
-      <c r="P28" s="45" t="s">
+      <c r="P28" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="Q28" s="46"/>
-      <c r="R28" s="46"/>
-      <c r="S28" s="46"/>
-      <c r="T28" s="46"/>
-      <c r="U28" s="46"/>
-      <c r="V28" s="47"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+      <c r="S28" s="56"/>
+      <c r="T28" s="56"/>
+      <c r="U28" s="56"/>
+      <c r="V28" s="57"/>
       <c r="X28" s="12"/>
       <c r="AD28" s="13"/>
-      <c r="AF28" s="51" t="s">
+      <c r="AF28" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="AG28" s="51"/>
-      <c r="AH28" s="51"/>
-      <c r="AI28" s="51"/>
-      <c r="AJ28" s="51"/>
-      <c r="AK28" s="51"/>
-      <c r="AL28" s="51"/>
+      <c r="AG28" s="45"/>
+      <c r="AH28" s="45"/>
+      <c r="AI28" s="45"/>
+      <c r="AJ28" s="45"/>
+      <c r="AK28" s="45"/>
+      <c r="AL28" s="45"/>
       <c r="AN28" s="12"/>
       <c r="AU28" s="8">
         <v>2</v>
@@ -3049,11 +3051,11 @@
       <c r="G30" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="I30" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52"/>
+      <c r="I30" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
       <c r="O30" s="12"/>
       <c r="P30" s="7">
         <v>1</v>
@@ -3103,11 +3105,11 @@
         <v>79</v>
       </c>
       <c r="AN30" s="12"/>
-      <c r="AQ30" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="AR30" s="52"/>
-      <c r="AS30" s="52"/>
+      <c r="AQ30" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR30" s="46"/>
+      <c r="AS30" s="46"/>
       <c r="AU30" s="38">
         <v>4</v>
       </c>
@@ -3402,15 +3404,15 @@
       <c r="BA33" s="6"/>
     </row>
     <row r="34" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="51"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
       <c r="L34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="8" t="s">
@@ -3459,15 +3461,15 @@
       </c>
       <c r="AN34" s="12"/>
       <c r="AQ34" s="12"/>
-      <c r="AU34" s="51" t="s">
+      <c r="AU34" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="AV34" s="51"/>
-      <c r="AW34" s="51"/>
-      <c r="AX34" s="51"/>
-      <c r="AY34" s="51"/>
-      <c r="AZ34" s="51"/>
-      <c r="BA34" s="51"/>
+      <c r="AV34" s="45"/>
+      <c r="AW34" s="45"/>
+      <c r="AX34" s="45"/>
+      <c r="AY34" s="45"/>
+      <c r="AZ34" s="45"/>
+      <c r="BA34" s="45"/>
     </row>
     <row r="35" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L35" s="12"/>
@@ -3520,20 +3522,20 @@
       <c r="AQ35" s="12"/>
     </row>
     <row r="36" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="51" t="s">
+      <c r="A36" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="L36" s="56" t="s">
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="L36" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="M36" s="52"/>
-      <c r="N36" s="52"/>
+      <c r="M36" s="46"/>
+      <c r="N36" s="46"/>
       <c r="O36" s="12"/>
       <c r="P36" s="8" t="s">
         <v>28</v>
@@ -3563,21 +3565,21 @@
       </c>
       <c r="AK36" s="36"/>
       <c r="AL36" s="37"/>
-      <c r="AN36" s="56" t="s">
+      <c r="AN36" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="AO36" s="52"/>
-      <c r="AP36" s="52"/>
+      <c r="AO36" s="46"/>
+      <c r="AP36" s="46"/>
       <c r="AQ36" s="12"/>
-      <c r="AU36" s="51" t="s">
+      <c r="AU36" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="AV36" s="51"/>
-      <c r="AW36" s="51"/>
-      <c r="AX36" s="51"/>
-      <c r="AY36" s="51"/>
-      <c r="AZ36" s="51"/>
-      <c r="BA36" s="51"/>
+      <c r="AV36" s="45"/>
+      <c r="AW36" s="45"/>
+      <c r="AX36" s="45"/>
+      <c r="AY36" s="45"/>
+      <c r="AZ36" s="45"/>
+      <c r="BA36" s="45"/>
     </row>
     <row r="37" spans="1:54" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="20" t="s">
@@ -3602,31 +3604,33 @@
         <v>25</v>
       </c>
       <c r="L37" s="12"/>
-      <c r="P37" s="48" t="s">
+      <c r="P37" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="Q37" s="49"/>
-      <c r="R37" s="49"/>
-      <c r="S37" s="49"/>
-      <c r="T37" s="49"/>
-      <c r="U37" s="49"/>
-      <c r="V37" s="50"/>
-      <c r="X37" s="56"/>
-      <c r="Y37" s="52"/>
-      <c r="Z37" s="52"/>
-      <c r="AA37" s="52"/>
-      <c r="AB37" s="52"/>
-      <c r="AC37" s="52"/>
-      <c r="AD37" s="60"/>
-      <c r="AF37" s="51" t="s">
+      <c r="Q37" s="59"/>
+      <c r="R37" s="59"/>
+      <c r="S37" s="59"/>
+      <c r="T37" s="59"/>
+      <c r="U37" s="59"/>
+      <c r="V37" s="60"/>
+      <c r="X37" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y37" s="46"/>
+      <c r="Z37" s="46"/>
+      <c r="AA37" s="46"/>
+      <c r="AB37" s="46"/>
+      <c r="AC37" s="46"/>
+      <c r="AD37" s="51"/>
+      <c r="AF37" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="AG37" s="51"/>
-      <c r="AH37" s="51"/>
-      <c r="AI37" s="51"/>
-      <c r="AJ37" s="51"/>
-      <c r="AK37" s="51"/>
-      <c r="AL37" s="51"/>
+      <c r="AG37" s="45"/>
+      <c r="AH37" s="45"/>
+      <c r="AI37" s="45"/>
+      <c r="AJ37" s="45"/>
+      <c r="AK37" s="45"/>
+      <c r="AL37" s="45"/>
       <c r="AQ37" s="12"/>
       <c r="AU37" s="3" t="s">
         <v>18</v>
@@ -3722,33 +3726,33 @@
         <v>59</v>
       </c>
       <c r="L39" s="12"/>
-      <c r="M39" s="45" t="s">
+      <c r="M39" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="N39" s="46"/>
-      <c r="O39" s="46"/>
-      <c r="P39" s="46"/>
-      <c r="Q39" s="46"/>
-      <c r="R39" s="46"/>
-      <c r="S39" s="47"/>
-      <c r="X39" s="51" t="s">
+      <c r="N39" s="56"/>
+      <c r="O39" s="56"/>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="56"/>
+      <c r="R39" s="56"/>
+      <c r="S39" s="57"/>
+      <c r="X39" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="Y39" s="51"/>
-      <c r="Z39" s="51"/>
-      <c r="AA39" s="51"/>
-      <c r="AB39" s="51"/>
-      <c r="AC39" s="51"/>
-      <c r="AD39" s="51"/>
-      <c r="AI39" s="51" t="s">
+      <c r="Y39" s="45"/>
+      <c r="Z39" s="45"/>
+      <c r="AA39" s="45"/>
+      <c r="AB39" s="45"/>
+      <c r="AC39" s="45"/>
+      <c r="AD39" s="45"/>
+      <c r="AI39" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="AJ39" s="51"/>
-      <c r="AK39" s="51"/>
-      <c r="AL39" s="51"/>
-      <c r="AM39" s="51"/>
-      <c r="AN39" s="51"/>
-      <c r="AO39" s="51"/>
+      <c r="AJ39" s="45"/>
+      <c r="AK39" s="45"/>
+      <c r="AL39" s="45"/>
+      <c r="AM39" s="45"/>
+      <c r="AN39" s="45"/>
+      <c r="AO39" s="45"/>
       <c r="AQ39" s="12"/>
       <c r="AU39" s="8">
         <v>2</v>
@@ -3906,11 +3910,11 @@
       <c r="G41" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="I41" s="52" t="s">
+      <c r="I41" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J41" s="52"/>
-      <c r="K41" s="52"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
       <c r="L41" s="12"/>
       <c r="M41" s="7">
         <v>1</v>
@@ -3978,11 +3982,11 @@
       <c r="AP41" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AQ41" s="56" t="s">
+      <c r="AQ41" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="AR41" s="52"/>
-      <c r="AS41" s="52"/>
+      <c r="AR41" s="46"/>
+      <c r="AS41" s="46"/>
       <c r="AU41" s="8">
         <v>4</v>
       </c>
@@ -4311,15 +4315,15 @@
       </c>
     </row>
     <row r="45" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
       <c r="M45" s="8" t="s">
         <v>27</v>
       </c>
@@ -4383,15 +4387,15 @@
       <c r="AO45" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="AU45" s="51" t="s">
+      <c r="AU45" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="AV45" s="51"/>
-      <c r="AW45" s="51"/>
-      <c r="AX45" s="51"/>
-      <c r="AY45" s="51"/>
-      <c r="AZ45" s="51"/>
-      <c r="BA45" s="51"/>
+      <c r="AV45" s="45"/>
+      <c r="AW45" s="45"/>
+      <c r="AX45" s="45"/>
+      <c r="AY45" s="45"/>
+      <c r="AZ45" s="45"/>
+      <c r="BA45" s="45"/>
     </row>
     <row r="46" spans="1:54" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="M46" s="8" t="s">
@@ -4484,12 +4488,18 @@
       <c r="Z47" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="AA47" s="15"/>
+      <c r="AA47" s="15">
+        <v>1</v>
+      </c>
       <c r="AB47" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="AC47" s="15"/>
-      <c r="AD47" s="6"/>
+      <c r="AC47" s="15">
+        <v>2</v>
+      </c>
+      <c r="AD47" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="AI47" s="9" t="s">
         <v>28</v>
       </c>
@@ -4505,49 +4515,61 @@
       <c r="AO47" s="6"/>
     </row>
     <row r="48" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M48" s="45" t="s">
+      <c r="M48" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="N48" s="46"/>
-      <c r="O48" s="46"/>
-      <c r="P48" s="46"/>
-      <c r="Q48" s="46"/>
-      <c r="R48" s="46"/>
-      <c r="S48" s="47"/>
-      <c r="X48" s="51" t="s">
+      <c r="N48" s="56"/>
+      <c r="O48" s="56"/>
+      <c r="P48" s="56"/>
+      <c r="Q48" s="56"/>
+      <c r="R48" s="56"/>
+      <c r="S48" s="57"/>
+      <c r="X48" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="Y48" s="51"/>
-      <c r="Z48" s="51"/>
-      <c r="AA48" s="51"/>
-      <c r="AB48" s="51"/>
-      <c r="AC48" s="51"/>
-      <c r="AD48" s="51"/>
-      <c r="AI48" s="51" t="s">
+      <c r="Y48" s="45"/>
+      <c r="Z48" s="45"/>
+      <c r="AA48" s="45"/>
+      <c r="AB48" s="45"/>
+      <c r="AC48" s="45"/>
+      <c r="AD48" s="45"/>
+      <c r="AI48" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="AJ48" s="51"/>
-      <c r="AK48" s="51"/>
-      <c r="AL48" s="51"/>
-      <c r="AM48" s="51"/>
-      <c r="AN48" s="51"/>
-      <c r="AO48" s="51"/>
+      <c r="AJ48" s="45"/>
+      <c r="AK48" s="45"/>
+      <c r="AL48" s="45"/>
+      <c r="AM48" s="45"/>
+      <c r="AN48" s="45"/>
+      <c r="AO48" s="45"/>
     </row>
     <row r="49" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="AU45:BA45"/>
-    <mergeCell ref="AF28:AL28"/>
-    <mergeCell ref="AF37:AL37"/>
-    <mergeCell ref="AQ30:AS30"/>
-    <mergeCell ref="AQ41:AS41"/>
-    <mergeCell ref="AU34:BA34"/>
-    <mergeCell ref="AU36:BA36"/>
-    <mergeCell ref="AU2:BA2"/>
-    <mergeCell ref="AU3:BA3"/>
-    <mergeCell ref="AU12:BA12"/>
-    <mergeCell ref="AU14:BA14"/>
-    <mergeCell ref="AU23:BA23"/>
+    <mergeCell ref="M48:S48"/>
+    <mergeCell ref="M39:S39"/>
+    <mergeCell ref="P37:V37"/>
+    <mergeCell ref="P28:V28"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="O26:W26"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="L36:N36"/>
+    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="M4:S4"/>
+    <mergeCell ref="M13:S13"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="A25:G25"/>
     <mergeCell ref="X37:AD37"/>
     <mergeCell ref="AE26:AM26"/>
     <mergeCell ref="Z1:AB1"/>
@@ -4564,121 +4586,109 @@
     <mergeCell ref="AN36:AP36"/>
     <mergeCell ref="AQ8:AS8"/>
     <mergeCell ref="AQ19:AS19"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="O26:W26"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="M2:R2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="M4:S4"/>
-    <mergeCell ref="M13:S13"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="M48:S48"/>
-    <mergeCell ref="M39:S39"/>
-    <mergeCell ref="P37:V37"/>
-    <mergeCell ref="P28:V28"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="AU2:BA2"/>
+    <mergeCell ref="AU3:BA3"/>
+    <mergeCell ref="AU12:BA12"/>
+    <mergeCell ref="AU14:BA14"/>
+    <mergeCell ref="AU23:BA23"/>
+    <mergeCell ref="AU45:BA45"/>
+    <mergeCell ref="AF28:AL28"/>
+    <mergeCell ref="AF37:AL37"/>
+    <mergeCell ref="AQ30:AS30"/>
+    <mergeCell ref="AQ41:AS41"/>
+    <mergeCell ref="AU34:BA34"/>
+    <mergeCell ref="AU36:BA36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="15">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$A$14:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C11 E5:E11 I8:K8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$A$20:$A$21</xm:f>
           </x14:formula1>
           <xm:sqref>C16:C22 E16:E22 I19:K19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$A$23:$A$24</xm:f>
           </x14:formula1>
           <xm:sqref>C27:C33 E27:E33 I30:K30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$A$17:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>C38:C44 E38:E44 I41:K41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$C$14:$C$15</xm:f>
           </x14:formula1>
           <xm:sqref>L14:N14 Q6:Q12 O6:O12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$C$17:$C$18</xm:f>
           </x14:formula1>
           <xm:sqref>L36:N36 Q41:Q47 O41:O47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$E$14:$E$15</xm:f>
           </x14:formula1>
           <xm:sqref>T30:T36 O26 R30:R36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$F$14:$F$15</xm:f>
           </x14:formula1>
           <xm:sqref>AE26:AM26 AJ30:AJ36 AH30:AH36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$G$13:$G$14</xm:f>
           </x14:formula1>
           <xm:sqref>X37:AD37 Z41:Z47 AB41:AB47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$B$14:$B$15</xm:f>
           </x14:formula1>
           <xm:sqref>AW5:AW11 AY5:AY11 AQ8:AS8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$B$20:$B$21</xm:f>
           </x14:formula1>
           <xm:sqref>AW16:AW22 AY16:AY22 AQ19:AS19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$B$23:$B$24</xm:f>
           </x14:formula1>
           <xm:sqref>AW27:AW33 AY27:AY33 AQ30:AS30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$B$17:$B$18</xm:f>
           </x14:formula1>
           <xm:sqref>AW38:AW44 AY38:AY44 AQ41:AS41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$D$14:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>AN14:AP14 AK5:AK11 AM5:AM11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000E000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Matchups!$D$17:$D$18</xm:f>
           </x14:formula1>

</xml_diff>